<commit_message>
adding R package NILC
</commit_message>
<xml_diff>
--- a/data/SupplementaryMaterial2.xlsx
+++ b/data/SupplementaryMaterial2.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/La meva unitat/NIG_ShareFolder/PanAf/TechPaper/PaperV5/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidhughes/Google Drive/work/writing/BCN/CF_tech_paper/Draft_v5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{110C65D9-3888-9A4B-9B78-A4CB9BE37513}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A4B3C00-B39D-194E-ADD7-B376E18A7328}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29160" yWindow="-2060" windowWidth="25600" windowHeight="15560" activeTab="4" xr2:uid="{C4FA65A5-49C4-D64F-9D2B-B8DBA5A1EE2A}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28580" windowHeight="18280" activeTab="2" xr2:uid="{C4FA65A5-49C4-D64F-9D2B-B8DBA5A1EE2A}"/>
   </bookViews>
   <sheets>
     <sheet name="Table S1" sheetId="4" r:id="rId1"/>
     <sheet name="Table S2" sheetId="5" r:id="rId2"/>
-    <sheet name="Table S4" sheetId="1" r:id="rId3"/>
-    <sheet name="Table S5" sheetId="6" r:id="rId4"/>
-    <sheet name="Downsampled" sheetId="9" r:id="rId5"/>
+    <sheet name="Table S3" sheetId="10" r:id="rId3"/>
+    <sheet name="Table S4" sheetId="1" r:id="rId4"/>
+    <sheet name="Table S5" sheetId="6" r:id="rId5"/>
+    <sheet name="Downsampled" sheetId="9" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3901" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3921" uniqueCount="417">
   <si>
     <t>P3E8</t>
   </si>
@@ -1269,6 +1270,24 @@
   <si>
     <t>Starting DNA (ug)</t>
   </si>
+  <si>
+    <t>Sites</t>
+  </si>
+  <si>
+    <t>Median Endogenous</t>
+  </si>
+  <si>
+    <t>Average Endogenous</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Ugalla</t>
+  </si>
 </sst>
 </file>
 
@@ -1278,7 +1297,7 @@
     <numFmt numFmtId="164" formatCode="0.00\ \X"/>
     <numFmt numFmtId="165" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1320,6 +1339,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1346,7 +1371,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -1484,6 +1509,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1491,7 +1545,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1581,19 +1635,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="20% - Accent6" xfId="3" builtinId="50"/>
     <cellStyle name="Accent1" xfId="2" builtinId="29"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="9">
     <dxf>
@@ -11446,6 +11518,296 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFA84E06-A145-1D42-B6AA-BC325EF5373A}">
+  <dimension ref="A1:E16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.5" customWidth="1"/>
+    <col min="2" max="2" width="25.5" customWidth="1"/>
+    <col min="3" max="3" width="22.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="31" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="74" t="s">
+        <v>411</v>
+      </c>
+      <c r="B1" s="75" t="s">
+        <v>412</v>
+      </c>
+      <c r="C1" s="76" t="s">
+        <v>413</v>
+      </c>
+      <c r="D1" s="75" t="s">
+        <v>414</v>
+      </c>
+      <c r="E1" s="75" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="77" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" s="78">
+        <v>0.7</v>
+      </c>
+      <c r="C2" s="79">
+        <v>1.1795</v>
+      </c>
+      <c r="D2" s="78">
+        <v>0.03</v>
+      </c>
+      <c r="E2" s="78">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="77" t="s">
+        <v>121</v>
+      </c>
+      <c r="B3" s="78">
+        <v>0.72</v>
+      </c>
+      <c r="C3" s="79">
+        <v>1.9875</v>
+      </c>
+      <c r="D3" s="78">
+        <v>0.05</v>
+      </c>
+      <c r="E3" s="78">
+        <v>9.42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="77" t="s">
+        <v>133</v>
+      </c>
+      <c r="B4" s="78">
+        <v>0</v>
+      </c>
+      <c r="C4" s="79">
+        <v>2.0899999999999998E-2</v>
+      </c>
+      <c r="D4" s="78">
+        <v>0</v>
+      </c>
+      <c r="E4" s="78">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="77" t="s">
+        <v>158</v>
+      </c>
+      <c r="B5" s="78">
+        <v>0.42</v>
+      </c>
+      <c r="C5" s="79">
+        <v>1.171</v>
+      </c>
+      <c r="D5" s="78">
+        <v>0</v>
+      </c>
+      <c r="E5" s="78">
+        <v>5.51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="77" t="s">
+        <v>176</v>
+      </c>
+      <c r="B6" s="78">
+        <v>0.22</v>
+      </c>
+      <c r="C6" s="79">
+        <v>2.5179999999999998</v>
+      </c>
+      <c r="D6" s="78">
+        <v>0</v>
+      </c>
+      <c r="E6" s="78">
+        <v>40.86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="77" t="s">
+        <v>193</v>
+      </c>
+      <c r="B7" s="78">
+        <v>0.94</v>
+      </c>
+      <c r="C7" s="79">
+        <v>1.2115</v>
+      </c>
+      <c r="D7" s="78">
+        <v>0.03</v>
+      </c>
+      <c r="E7" s="78">
+        <v>3.68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="77" t="s">
+        <v>213</v>
+      </c>
+      <c r="B8" s="78">
+        <v>0.60499999999999998</v>
+      </c>
+      <c r="C8" s="79">
+        <v>0.94299999999999995</v>
+      </c>
+      <c r="D8" s="78">
+        <v>0.02</v>
+      </c>
+      <c r="E8" s="78">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="77" t="s">
+        <v>226</v>
+      </c>
+      <c r="B9" s="78">
+        <v>0.45</v>
+      </c>
+      <c r="C9" s="79">
+        <v>0.88100000000000001</v>
+      </c>
+      <c r="D9" s="78">
+        <v>0.04</v>
+      </c>
+      <c r="E9" s="78">
+        <v>3.32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="77" t="s">
+        <v>242</v>
+      </c>
+      <c r="B10" s="78">
+        <v>0.105</v>
+      </c>
+      <c r="C10" s="79">
+        <v>0.41299999999999998</v>
+      </c>
+      <c r="D10" s="78">
+        <v>0.01</v>
+      </c>
+      <c r="E10" s="78">
+        <v>2.86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="77" t="s">
+        <v>262</v>
+      </c>
+      <c r="B11" s="78">
+        <v>0.17</v>
+      </c>
+      <c r="C11" s="79">
+        <v>0.98799999999999999</v>
+      </c>
+      <c r="D11" s="78">
+        <v>0.02</v>
+      </c>
+      <c r="E11" s="78">
+        <v>6.68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="77" t="s">
+        <v>280</v>
+      </c>
+      <c r="B12" s="78">
+        <v>1.58</v>
+      </c>
+      <c r="C12" s="79">
+        <v>6.9595000000000002</v>
+      </c>
+      <c r="D12" s="78">
+        <v>0.05</v>
+      </c>
+      <c r="E12" s="78">
+        <v>47.57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="77" t="s">
+        <v>301</v>
+      </c>
+      <c r="B13" s="78">
+        <v>0.15</v>
+      </c>
+      <c r="C13" s="79">
+        <v>0.8155</v>
+      </c>
+      <c r="D13" s="78">
+        <v>0</v>
+      </c>
+      <c r="E13" s="78">
+        <v>6.31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="77" t="s">
+        <v>319</v>
+      </c>
+      <c r="B14" s="78">
+        <v>0.215</v>
+      </c>
+      <c r="C14" s="79">
+        <v>0.50249999999999995</v>
+      </c>
+      <c r="D14" s="78">
+        <v>0</v>
+      </c>
+      <c r="E14" s="78">
+        <v>4.45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="77" t="s">
+        <v>335</v>
+      </c>
+      <c r="B15" s="78">
+        <v>0.47</v>
+      </c>
+      <c r="C15" s="79">
+        <v>1.484</v>
+      </c>
+      <c r="D15" s="78">
+        <v>0.01</v>
+      </c>
+      <c r="E15" s="78">
+        <v>6.9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="77" t="s">
+        <v>416</v>
+      </c>
+      <c r="B16" s="78">
+        <v>1.17</v>
+      </c>
+      <c r="C16" s="79">
+        <v>1.4079999999999999</v>
+      </c>
+      <c r="D16" s="78">
+        <v>0.03</v>
+      </c>
+      <c r="E16" s="78">
+        <v>3.85</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E416726-80F5-AE4F-8C9B-CE172F709620}">
   <dimension ref="A1:X404"/>
   <sheetViews>
@@ -40580,7 +40942,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46FD8B2C-2758-5D44-96A5-A08ECD1C51F2}">
   <dimension ref="A1:L19"/>
   <sheetViews>
@@ -40625,10 +40987,10 @@
       <c r="J1" s="57" t="s">
         <v>373</v>
       </c>
-      <c r="K1" s="71" t="s">
+      <c r="K1" s="72" t="s">
         <v>374</v>
       </c>
-      <c r="L1" s="72"/>
+      <c r="L1" s="73"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="60" t="s">
@@ -41322,11 +41684,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DC2C328-E155-5C46-B060-31CA9DBD4BF6}">
   <dimension ref="A1:Y389"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -41488,7 +41850,7 @@
       <c r="X2">
         <v>2.9195279411159999E-4</v>
       </c>
-      <c r="Y2" s="73">
+      <c r="Y2" s="71">
         <v>4.9344134216045098E-5</v>
       </c>
     </row>
@@ -41565,7 +41927,7 @@
       <c r="X3">
         <v>3.5363296188165602E-4</v>
       </c>
-      <c r="Y3" s="73">
+      <c r="Y3" s="71">
         <v>7.4016201324067596E-5</v>
       </c>
     </row>
@@ -41642,7 +42004,7 @@
       <c r="X4">
         <v>2.6728072700357702E-4</v>
       </c>
-      <c r="Y4" s="73">
+      <c r="Y4" s="71">
         <v>3.7008100662033798E-5</v>
       </c>
     </row>
@@ -41716,10 +42078,10 @@
       <c r="W5">
         <v>1.11024301986101E-4</v>
       </c>
-      <c r="X5" s="73">
+      <c r="X5" s="71">
         <v>2.8784078292693002E-5</v>
       </c>
-      <c r="Y5" s="73">
+      <c r="Y5" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -41796,7 +42158,7 @@
       <c r="X6">
         <v>2.6316871581890701E-4</v>
       </c>
-      <c r="Y6" s="73">
+      <c r="Y6" s="71">
         <v>2.8784078292693002E-5</v>
       </c>
     </row>
@@ -41873,7 +42235,7 @@
       <c r="X7">
         <v>5.4278547637649603E-4</v>
       </c>
-      <c r="Y7" s="73">
+      <c r="Y7" s="71">
         <v>4.9344134216045098E-5</v>
       </c>
     </row>
@@ -41944,13 +42306,13 @@
       <c r="V8">
         <v>8.8408240470414098E-4</v>
       </c>
-      <c r="W8" s="73">
+      <c r="W8" s="71">
         <v>4.9344134216045098E-5</v>
       </c>
-      <c r="X8" s="73">
+      <c r="X8" s="71">
         <v>1.23360335540113E-5</v>
       </c>
-      <c r="Y8" s="73">
+      <c r="Y8" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -42024,7 +42386,7 @@
       <c r="W9">
         <v>3.2073687240429303E-4</v>
       </c>
-      <c r="X9" s="73">
+      <c r="X9" s="71">
         <v>8.22402236934084E-5</v>
       </c>
       <c r="Y9">
@@ -42104,7 +42466,7 @@
       <c r="X10">
         <v>2.2616061515687299E-4</v>
       </c>
-      <c r="Y10" s="73">
+      <c r="Y10" s="71">
         <v>4.11201118467042E-5</v>
       </c>
     </row>
@@ -42181,7 +42543,7 @@
       <c r="X11">
         <v>4.8932933097578003E-4</v>
       </c>
-      <c r="Y11" s="73">
+      <c r="Y11" s="71">
         <v>6.9904190139397201E-5</v>
       </c>
     </row>
@@ -42255,10 +42617,10 @@
       <c r="W12">
         <v>3.7830502898967899E-4</v>
       </c>
-      <c r="X12" s="73">
+      <c r="X12" s="71">
         <v>9.4576257247419706E-5</v>
       </c>
-      <c r="Y12" s="73">
+      <c r="Y12" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -42332,10 +42694,10 @@
       <c r="W13">
         <v>3.9064106254369001E-4</v>
       </c>
-      <c r="X13" s="73">
+      <c r="X13" s="71">
         <v>8.22402236934084E-5</v>
       </c>
-      <c r="Y13" s="73">
+      <c r="Y13" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -42409,10 +42771,10 @@
       <c r="W14">
         <v>3.5774497306632701E-4</v>
       </c>
-      <c r="X14" s="73">
+      <c r="X14" s="71">
         <v>9.8688268432090101E-5</v>
       </c>
-      <c r="Y14" s="73">
+      <c r="Y14" s="71">
         <v>1.23360335540113E-5</v>
       </c>
     </row>
@@ -42486,7 +42848,7 @@
       <c r="W15">
         <v>1.4392039146346499E-4</v>
       </c>
-      <c r="X15" s="73">
+      <c r="X15" s="71">
         <v>3.7008100662033798E-5</v>
       </c>
       <c r="Y15">
@@ -42566,7 +42928,7 @@
       <c r="X16">
         <v>1.3569636909412401E-4</v>
       </c>
-      <c r="Y16" s="73">
+      <c r="Y16" s="71">
         <v>1.6448044738681702E-5</v>
       </c>
     </row>
@@ -42643,7 +43005,7 @@
       <c r="X17">
         <v>3.82417040174349E-4</v>
       </c>
-      <c r="Y17" s="73">
+      <c r="Y17" s="71">
         <v>2.05600559233521E-5</v>
       </c>
     </row>
@@ -42717,10 +43079,10 @@
       <c r="W18">
         <v>4.1531312965171298E-4</v>
       </c>
-      <c r="X18" s="73">
+      <c r="X18" s="71">
         <v>9.8688268432090101E-5</v>
       </c>
-      <c r="Y18" s="73">
+      <c r="Y18" s="71">
         <v>1.23360335540113E-5</v>
       </c>
     </row>
@@ -42797,7 +43159,7 @@
       <c r="X19">
         <v>1.60368436202146E-4</v>
       </c>
-      <c r="Y19" s="73">
+      <c r="Y19" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -42868,10 +43230,10 @@
       <c r="V20">
         <v>3.0428882766561101E-4</v>
       </c>
-      <c r="W20" s="73">
+      <c r="W20" s="71">
         <v>2.4672067108022502E-5</v>
       </c>
-      <c r="X20" s="73">
+      <c r="X20" s="71">
         <v>1.23360335540113E-5</v>
       </c>
       <c r="Y20">
@@ -42945,10 +43307,10 @@
       <c r="V21">
         <v>1.65302849623751E-3</v>
       </c>
-      <c r="W21" s="73">
+      <c r="W21" s="71">
         <v>9.4576257247419706E-5</v>
       </c>
-      <c r="X21" s="73">
+      <c r="X21" s="71">
         <v>1.23360335540113E-5</v>
       </c>
       <c r="Y21">
@@ -43028,7 +43390,7 @@
       <c r="X22">
         <v>3.08400838850282E-4</v>
       </c>
-      <c r="Y22" s="73">
+      <c r="Y22" s="71">
         <v>4.5232123031374602E-5</v>
       </c>
     </row>
@@ -43102,10 +43464,10 @@
       <c r="W23">
         <v>2.8784078292692997E-4</v>
       </c>
-      <c r="X23" s="73">
+      <c r="X23" s="71">
         <v>7.8128212508738005E-5</v>
       </c>
-      <c r="Y23" s="73">
+      <c r="Y23" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -43182,7 +43544,7 @@
       <c r="X24">
         <v>3.4540893951231502E-4</v>
       </c>
-      <c r="Y24" s="73">
+      <c r="Y24" s="71">
         <v>9.8688268432090101E-5</v>
       </c>
     </row>
@@ -43256,10 +43618,10 @@
       <c r="W25">
         <v>1.7681648094082801E-4</v>
       </c>
-      <c r="X25" s="73">
+      <c r="X25" s="71">
         <v>4.5232123031374602E-5</v>
       </c>
-      <c r="Y25" s="73">
+      <c r="Y25" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -43336,7 +43698,7 @@
       <c r="X26">
         <v>2.4260865989555501E-4</v>
       </c>
-      <c r="Y26" s="73">
+      <c r="Y26" s="71">
         <v>2.4672067108022502E-5</v>
       </c>
     </row>
@@ -43410,10 +43772,10 @@
       <c r="W27">
         <v>6.6203380073193803E-4</v>
       </c>
-      <c r="X27" s="73">
+      <c r="X27" s="71">
         <v>6.1680167770056303E-5</v>
       </c>
-      <c r="Y27" s="73">
+      <c r="Y27" s="71">
         <v>1.6448044738681702E-5</v>
       </c>
     </row>
@@ -43484,13 +43846,13 @@
       <c r="V28">
         <v>1.2336033554011301E-4</v>
       </c>
-      <c r="W28" s="73">
+      <c r="W28" s="71">
         <v>4.11201118467042E-5</v>
       </c>
-      <c r="X28" s="73">
+      <c r="X28" s="71">
         <v>2.05600559233521E-5</v>
       </c>
-      <c r="Y28" s="73">
+      <c r="Y28" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -43564,10 +43926,10 @@
       <c r="W29">
         <v>1.6448044738681699E-4</v>
       </c>
-      <c r="X29" s="73">
+      <c r="X29" s="71">
         <v>1.23360335540113E-5</v>
       </c>
-      <c r="Y29" s="73">
+      <c r="Y29" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -43721,7 +44083,7 @@
       <c r="X31">
         <v>2.7550474937291798E-4</v>
       </c>
-      <c r="Y31" s="73">
+      <c r="Y31" s="71">
         <v>7.4016201324067596E-5</v>
       </c>
     </row>
@@ -43795,10 +44157,10 @@
       <c r="W32">
         <v>3.74193017805008E-4</v>
       </c>
-      <c r="X32" s="73">
+      <c r="X32" s="71">
         <v>9.4576257247419706E-5</v>
       </c>
-      <c r="Y32" s="73">
+      <c r="Y32" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -43872,10 +44234,10 @@
       <c r="W33">
         <v>3.9064106254369001E-4</v>
       </c>
-      <c r="X33" s="73">
+      <c r="X33" s="71">
         <v>8.22402236934084E-5</v>
       </c>
-      <c r="Y33" s="73">
+      <c r="Y33" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -43949,10 +44311,10 @@
       <c r="W34">
         <v>3.3307290595830399E-4</v>
       </c>
-      <c r="X34" s="73">
+      <c r="X34" s="71">
         <v>9.0464246062749298E-5</v>
       </c>
-      <c r="Y34" s="73">
+      <c r="Y34" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -44026,7 +44388,7 @@
       <c r="W35">
         <v>1.68592458571487E-4</v>
       </c>
-      <c r="X35" s="73">
+      <c r="X35" s="71">
         <v>3.2896089477363403E-5</v>
       </c>
       <c r="Y35">
@@ -44106,7 +44468,7 @@
       <c r="X36">
         <v>1.39808380278794E-4</v>
       </c>
-      <c r="Y36" s="73">
+      <c r="Y36" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -44183,7 +44545,7 @@
       <c r="X37">
         <v>3.6185698425099697E-4</v>
       </c>
-      <c r="Y37" s="73">
+      <c r="Y37" s="71">
         <v>2.4672067108022502E-5</v>
       </c>
     </row>
@@ -44257,10 +44619,10 @@
       <c r="W38">
         <v>3.41296928327645E-4</v>
       </c>
-      <c r="X38" s="73">
+      <c r="X38" s="71">
         <v>7.8128212508738005E-5</v>
       </c>
-      <c r="Y38" s="73">
+      <c r="Y38" s="71">
         <v>1.23360335540113E-5</v>
       </c>
     </row>
@@ -44337,7 +44699,7 @@
       <c r="X39">
         <v>1.68592458571487E-4</v>
       </c>
-      <c r="Y39" s="73">
+      <c r="Y39" s="71">
         <v>1.23360335540113E-5</v>
       </c>
     </row>
@@ -44408,10 +44770,10 @@
       <c r="V40">
         <v>3.00176816480941E-4</v>
       </c>
-      <c r="W40" s="73">
+      <c r="W40" s="71">
         <v>3.2896089477363403E-5</v>
       </c>
-      <c r="X40" s="73">
+      <c r="X40" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
       <c r="Y40">
@@ -44488,7 +44850,7 @@
       <c r="W41">
         <v>1.02800279616761E-4</v>
       </c>
-      <c r="X41" s="73">
+      <c r="X41" s="71">
         <v>1.6448044738681702E-5</v>
       </c>
       <c r="Y41">
@@ -44568,7 +44930,7 @@
       <c r="X42">
         <v>2.8372877174225898E-4</v>
       </c>
-      <c r="Y42" s="73">
+      <c r="Y42" s="71">
         <v>3.2896089477363403E-5</v>
       </c>
     </row>
@@ -44642,7 +45004,7 @@
       <c r="W43">
         <v>2.9195279411159999E-4</v>
       </c>
-      <c r="X43" s="73">
+      <c r="X43" s="71">
         <v>7.8128212508738005E-5</v>
       </c>
       <c r="Y43">
@@ -44722,7 +45084,7 @@
       <c r="X44">
         <v>3.4952095069698601E-4</v>
       </c>
-      <c r="Y44" s="73">
+      <c r="Y44" s="71">
         <v>8.6352234878078903E-5</v>
       </c>
     </row>
@@ -44796,10 +45158,10 @@
       <c r="W45">
         <v>1.5625642501747601E-4</v>
       </c>
-      <c r="X45" s="73">
+      <c r="X45" s="71">
         <v>4.9344134216045098E-5</v>
       </c>
-      <c r="Y45" s="73">
+      <c r="Y45" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -44876,7 +45238,7 @@
       <c r="X46">
         <v>2.3849664871088499E-4</v>
       </c>
-      <c r="Y46" s="73">
+      <c r="Y46" s="71">
         <v>2.4672067108022502E-5</v>
       </c>
     </row>
@@ -44950,10 +45312,10 @@
       <c r="W47">
         <v>5.7156955466918901E-4</v>
       </c>
-      <c r="X47" s="73">
+      <c r="X47" s="71">
         <v>6.1680167770056303E-5</v>
       </c>
-      <c r="Y47" s="73">
+      <c r="Y47" s="71">
         <v>2.05600559233521E-5</v>
       </c>
     </row>
@@ -45024,13 +45386,13 @@
       <c r="V48">
         <v>1.11024301986101E-4</v>
       </c>
-      <c r="W48" s="73">
+      <c r="W48" s="71">
         <v>3.7008100662033798E-5</v>
       </c>
-      <c r="X48" s="73">
+      <c r="X48" s="71">
         <v>2.4672067108022502E-5</v>
       </c>
-      <c r="Y48" s="73">
+      <c r="Y48" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -45104,10 +45466,10 @@
       <c r="W49">
         <v>1.72704469756158E-4</v>
       </c>
-      <c r="X49" s="73">
+      <c r="X49" s="71">
         <v>1.6448044738681702E-5</v>
       </c>
-      <c r="Y49" s="73">
+      <c r="Y49" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -45261,7 +45623,7 @@
       <c r="X51">
         <v>2.6316871581890701E-4</v>
       </c>
-      <c r="Y51" s="73">
+      <c r="Y51" s="71">
         <v>8.22402236934084E-5</v>
       </c>
     </row>
@@ -45335,10 +45697,10 @@
       <c r="W52">
         <v>1.68592458571487E-4</v>
       </c>
-      <c r="X52" s="73">
+      <c r="X52" s="71">
         <v>2.05600559233521E-5</v>
       </c>
-      <c r="Y52" s="73">
+      <c r="Y52" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -45412,10 +45774,10 @@
       <c r="W53">
         <v>2.34384637526214E-4</v>
       </c>
-      <c r="X53" s="73">
+      <c r="X53" s="71">
         <v>4.5232123031374602E-5</v>
       </c>
-      <c r="Y53" s="73">
+      <c r="Y53" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -45492,7 +45854,7 @@
       <c r="X54">
         <v>1.5214441383280599E-4</v>
       </c>
-      <c r="Y54" s="73">
+      <c r="Y54" s="71">
         <v>1.23360335540113E-5</v>
       </c>
     </row>
@@ -45563,10 +45925,10 @@
       <c r="V55">
         <v>8.4296229285743703E-4</v>
       </c>
-      <c r="W55" s="73">
+      <c r="W55" s="71">
         <v>6.9904190139397201E-5</v>
       </c>
-      <c r="X55" s="73">
+      <c r="X55" s="71">
         <v>1.23360335540113E-5</v>
       </c>
       <c r="Y55">
@@ -45643,10 +46005,10 @@
       <c r="W56">
         <v>1.72704469756158E-4</v>
       </c>
-      <c r="X56" s="73">
+      <c r="X56" s="71">
         <v>1.6448044738681702E-5</v>
       </c>
-      <c r="Y56" s="73">
+      <c r="Y56" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -45723,7 +46085,7 @@
       <c r="X57">
         <v>1.06912290801431E-4</v>
       </c>
-      <c r="Y57" s="73">
+      <c r="Y57" s="71">
         <v>1.23360335540113E-5</v>
       </c>
     </row>
@@ -45800,7 +46162,7 @@
       <c r="X58">
         <v>1.6448044738681699E-4</v>
       </c>
-      <c r="Y58" s="73">
+      <c r="Y58" s="71">
         <v>1.23360335540113E-5</v>
       </c>
     </row>
@@ -45874,10 +46236,10 @@
       <c r="W59">
         <v>1.80928492125499E-4</v>
       </c>
-      <c r="X59" s="73">
+      <c r="X59" s="71">
         <v>2.8784078292693002E-5</v>
       </c>
-      <c r="Y59" s="73">
+      <c r="Y59" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -45951,10 +46313,10 @@
       <c r="W60">
         <v>2.2204860397220301E-4</v>
       </c>
-      <c r="X60" s="73">
+      <c r="X60" s="71">
         <v>3.2896089477363403E-5</v>
       </c>
-      <c r="Y60" s="73">
+      <c r="Y60" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -46031,7 +46393,7 @@
       <c r="X61">
         <v>1.6448044738681699E-4</v>
       </c>
-      <c r="Y61" s="73">
+      <c r="Y61" s="71">
         <v>1.23360335540113E-5</v>
       </c>
     </row>
@@ -46108,7 +46470,7 @@
       <c r="X62">
         <v>1.3158435790945399E-4</v>
       </c>
-      <c r="Y62" s="73">
+      <c r="Y62" s="71">
         <v>1.23360335540113E-5</v>
       </c>
     </row>
@@ -46182,10 +46544,10 @@
       <c r="W63">
         <v>4.7699329742176901E-4</v>
       </c>
-      <c r="X63" s="73">
+      <c r="X63" s="71">
         <v>6.1680167770056303E-5</v>
       </c>
-      <c r="Y63" s="73">
+      <c r="Y63" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -46259,10 +46621,10 @@
       <c r="W64">
         <v>1.8504050331016899E-4</v>
       </c>
-      <c r="X64" s="73">
+      <c r="X64" s="71">
         <v>6.9904190139397201E-5</v>
       </c>
-      <c r="Y64" s="73">
+      <c r="Y64" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -46336,10 +46698,10 @@
       <c r="W65">
         <v>4.8932933097578003E-4</v>
       </c>
-      <c r="X65" s="73">
+      <c r="X65" s="71">
         <v>9.8688268432090101E-5</v>
       </c>
-      <c r="Y65" s="73">
+      <c r="Y65" s="71">
         <v>1.23360335540113E-5</v>
       </c>
     </row>
@@ -46413,10 +46775,10 @@
       <c r="W66">
         <v>3.7008100662033798E-4</v>
       </c>
-      <c r="X66" s="73">
+      <c r="X66" s="71">
         <v>9.0464246062749298E-5</v>
       </c>
-      <c r="Y66" s="73">
+      <c r="Y66" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -46490,10 +46852,10 @@
       <c r="W67">
         <v>3.7008100662033798E-4</v>
       </c>
-      <c r="X67" s="73">
+      <c r="X67" s="71">
         <v>6.9904190139397201E-5</v>
       </c>
-      <c r="Y67" s="73">
+      <c r="Y67" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -46570,7 +46932,7 @@
       <c r="X68">
         <v>1.3158435790945399E-4</v>
       </c>
-      <c r="Y68" s="73">
+      <c r="Y68" s="71">
         <v>2.4672067108022502E-5</v>
       </c>
     </row>
@@ -46644,10 +47006,10 @@
       <c r="W69">
         <v>2.4260865989555501E-4</v>
       </c>
-      <c r="X69" s="73">
+      <c r="X69" s="71">
         <v>4.11201118467042E-5</v>
       </c>
-      <c r="Y69" s="73">
+      <c r="Y69" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -46721,10 +47083,10 @@
       <c r="W70">
         <v>2.0560055923352099E-4</v>
       </c>
-      <c r="X70" s="73">
+      <c r="X70" s="71">
         <v>6.1680167770056303E-5</v>
       </c>
-      <c r="Y70" s="73">
+      <c r="Y70" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -46798,10 +47160,10 @@
       <c r="W71">
         <v>2.0971257041819201E-4</v>
       </c>
-      <c r="X71" s="73">
+      <c r="X71" s="71">
         <v>4.9344134216045098E-5</v>
       </c>
-      <c r="Y71" s="73">
+      <c r="Y71" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -46878,7 +47240,7 @@
       <c r="X72">
         <v>1.80928492125499E-4</v>
       </c>
-      <c r="Y72" s="73">
+      <c r="Y72" s="71">
         <v>1.6448044738681702E-5</v>
       </c>
     </row>
@@ -46952,10 +47314,10 @@
       <c r="W73">
         <v>4.3176117439039401E-4</v>
       </c>
-      <c r="X73" s="73">
+      <c r="X73" s="71">
         <v>8.22402236934084E-5</v>
       </c>
-      <c r="Y73" s="73">
+      <c r="Y73" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -47029,10 +47391,10 @@
       <c r="W74">
         <v>2.2204860397220301E-4</v>
       </c>
-      <c r="X74" s="73">
+      <c r="X74" s="71">
         <v>3.2896089477363403E-5</v>
       </c>
-      <c r="Y74" s="73">
+      <c r="Y74" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -47109,7 +47471,7 @@
       <c r="X75">
         <v>1.11024301986101E-4</v>
       </c>
-      <c r="Y75" s="73">
+      <c r="Y75" s="71">
         <v>1.23360335540113E-5</v>
       </c>
     </row>
@@ -47183,10 +47545,10 @@
       <c r="W76">
         <v>2.0971257041819201E-4</v>
       </c>
-      <c r="X76" s="73">
+      <c r="X76" s="71">
         <v>8.6352234878078903E-5</v>
       </c>
-      <c r="Y76" s="73">
+      <c r="Y76" s="71">
         <v>2.8784078292693002E-5</v>
       </c>
     </row>
@@ -47337,10 +47699,10 @@
       <c r="W78">
         <v>2.5905670463423699E-4</v>
       </c>
-      <c r="X78" s="73">
+      <c r="X78" s="71">
         <v>7.4016201324067596E-5</v>
       </c>
-      <c r="Y78" s="73">
+      <c r="Y78" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -47414,10 +47776,10 @@
       <c r="W79">
         <v>1.80928492125499E-4</v>
       </c>
-      <c r="X79" s="73">
+      <c r="X79" s="71">
         <v>3.7008100662033798E-5</v>
       </c>
-      <c r="Y79" s="73">
+      <c r="Y79" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -47488,10 +47850,10 @@
       <c r="V80">
         <v>3.5774497306632701E-4</v>
       </c>
-      <c r="W80" s="73">
+      <c r="W80" s="71">
         <v>3.7008100662033798E-5</v>
       </c>
-      <c r="X80" s="73">
+      <c r="X80" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
       <c r="Y80">
@@ -47568,10 +47930,10 @@
       <c r="W81">
         <v>3.2896089477363398E-4</v>
       </c>
-      <c r="X81" s="73">
+      <c r="X81" s="71">
         <v>4.9344134216045098E-5</v>
       </c>
-      <c r="Y81" s="73">
+      <c r="Y81" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -47645,10 +48007,10 @@
       <c r="W82">
         <v>1.11024301986101E-4</v>
       </c>
-      <c r="X82" s="73">
+      <c r="X82" s="71">
         <v>1.23360335540113E-5</v>
       </c>
-      <c r="Y82" s="73">
+      <c r="Y82" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -47722,10 +48084,10 @@
       <c r="W83">
         <v>1.06912290801431E-4</v>
       </c>
-      <c r="X83" s="73">
+      <c r="X83" s="71">
         <v>1.6448044738681702E-5</v>
       </c>
-      <c r="Y83" s="73">
+      <c r="Y83" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -47799,10 +48161,10 @@
       <c r="W84">
         <v>3.94753073728361E-4</v>
       </c>
-      <c r="X84" s="73">
+      <c r="X84" s="71">
         <v>9.0464246062749298E-5</v>
       </c>
-      <c r="Y84" s="73">
+      <c r="Y84" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -47873,10 +48235,10 @@
       <c r="V85">
         <v>2.2616061515687299E-4</v>
       </c>
-      <c r="W85" s="73">
+      <c r="W85" s="71">
         <v>3.2896089477363403E-5</v>
       </c>
-      <c r="X85" s="73">
+      <c r="X85" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
       <c r="Y85">
@@ -47950,13 +48312,13 @@
       <c r="V86">
         <v>1.06501089682964E-3</v>
       </c>
-      <c r="W86" s="73">
+      <c r="W86" s="71">
         <v>5.7568156585385901E-5</v>
       </c>
-      <c r="X86" s="73">
+      <c r="X86" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
-      <c r="Y86" s="73">
+      <c r="Y86" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -48030,10 +48392,10 @@
       <c r="W87">
         <v>3.74193017805008E-4</v>
       </c>
-      <c r="X87" s="73">
+      <c r="X87" s="71">
         <v>5.34561454007155E-5</v>
       </c>
-      <c r="Y87" s="73">
+      <c r="Y87" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -48110,7 +48472,7 @@
       <c r="X88">
         <v>1.3158435790945399E-4</v>
       </c>
-      <c r="Y88" s="73">
+      <c r="Y88" s="71">
         <v>1.23360335540113E-5</v>
       </c>
     </row>
@@ -48184,10 +48546,10 @@
       <c r="W89">
         <v>1.5625642501747601E-4</v>
       </c>
-      <c r="X89" s="73">
+      <c r="X89" s="71">
         <v>2.05600559233521E-5</v>
       </c>
-      <c r="Y89" s="73">
+      <c r="Y89" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -48261,7 +48623,7 @@
       <c r="W90">
         <v>1.48032402648135E-4</v>
       </c>
-      <c r="X90" s="73">
+      <c r="X90" s="71">
         <v>3.2896089477363403E-5</v>
       </c>
       <c r="Y90">
@@ -48338,10 +48700,10 @@
       <c r="W91">
         <v>5.5100949874583704E-4</v>
       </c>
-      <c r="X91" s="73">
+      <c r="X91" s="71">
         <v>9.4576257247419706E-5</v>
       </c>
-      <c r="Y91" s="73">
+      <c r="Y91" s="71">
         <v>1.23360335540113E-5</v>
       </c>
     </row>
@@ -48415,10 +48777,10 @@
       <c r="W92">
         <v>4.7288128623709899E-4</v>
       </c>
-      <c r="X92" s="73">
+      <c r="X92" s="71">
         <v>7.8128212508738005E-5</v>
       </c>
-      <c r="Y92" s="73">
+      <c r="Y92" s="71">
         <v>1.23360335540113E-5</v>
       </c>
     </row>
@@ -48489,10 +48851,10 @@
       <c r="V93">
         <v>1.0197787737982601E-3</v>
       </c>
-      <c r="W93" s="73">
+      <c r="W93" s="71">
         <v>8.22402236934084E-5</v>
       </c>
-      <c r="X93" s="73">
+      <c r="X93" s="71">
         <v>1.6448044738681702E-5</v>
       </c>
       <c r="Y93">
@@ -48569,7 +48931,7 @@
       <c r="W94">
         <v>1.3569636909412401E-4</v>
       </c>
-      <c r="X94" s="73">
+      <c r="X94" s="71">
         <v>3.7008100662033798E-5</v>
       </c>
       <c r="Y94">
@@ -48646,10 +49008,10 @@
       <c r="W95">
         <v>3.08400838850282E-4</v>
       </c>
-      <c r="X95" s="73">
+      <c r="X95" s="71">
         <v>6.5792178954726806E-5</v>
       </c>
-      <c r="Y95" s="73">
+      <c r="Y95" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -48723,10 +49085,10 @@
       <c r="W96">
         <v>3.4540893951231502E-4</v>
       </c>
-      <c r="X96" s="73">
+      <c r="X96" s="71">
         <v>7.4016201324067596E-5</v>
       </c>
-      <c r="Y96" s="73">
+      <c r="Y96" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -48800,7 +49162,7 @@
       <c r="W97">
         <v>2.0971257041819201E-4</v>
       </c>
-      <c r="X97" s="73">
+      <c r="X97" s="71">
         <v>4.9344134216045098E-5</v>
       </c>
       <c r="Y97">
@@ -48880,7 +49242,7 @@
       <c r="X98">
         <v>1.27472346724783E-4</v>
       </c>
-      <c r="Y98" s="73">
+      <c r="Y98" s="71">
         <v>1.6448044738681702E-5</v>
       </c>
     </row>
@@ -48951,13 +49313,13 @@
       <c r="V99">
         <v>5.8390558822319998E-4</v>
       </c>
-      <c r="W99" s="73">
+      <c r="W99" s="71">
         <v>5.7568156585385901E-5</v>
       </c>
-      <c r="X99" s="73">
+      <c r="X99" s="71">
         <v>2.05600559233521E-5</v>
       </c>
-      <c r="Y99" s="73">
+      <c r="Y99" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -49031,10 +49393,10 @@
       <c r="W100">
         <v>1.1924832435544199E-4</v>
       </c>
-      <c r="X100" s="73">
+      <c r="X100" s="71">
         <v>2.05600559233521E-5</v>
       </c>
-      <c r="Y100" s="73">
+      <c r="Y100" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -49108,10 +49470,10 @@
       <c r="W101">
         <v>1.80928492125499E-4</v>
       </c>
-      <c r="X101" s="73">
+      <c r="X101" s="71">
         <v>2.05600559233521E-5</v>
       </c>
-      <c r="Y101" s="73">
+      <c r="Y101" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -49188,7 +49550,7 @@
       <c r="X102">
         <v>1.5625642501747601E-4</v>
       </c>
-      <c r="Y102" s="73">
+      <c r="Y102" s="71">
         <v>1.6448044738681702E-5</v>
       </c>
     </row>
@@ -49262,10 +49624,10 @@
       <c r="W103">
         <v>3.1662486121962301E-4</v>
       </c>
-      <c r="X103" s="73">
+      <c r="X103" s="71">
         <v>6.5792178954726806E-5</v>
       </c>
-      <c r="Y103" s="73">
+      <c r="Y103" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -49339,10 +49701,10 @@
       <c r="W104">
         <v>1.3158435790945399E-4</v>
       </c>
-      <c r="X104" s="73">
+      <c r="X104" s="71">
         <v>1.6448044738681702E-5</v>
       </c>
-      <c r="Y104" s="73">
+      <c r="Y104" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -49419,7 +49781,7 @@
       <c r="X105">
         <v>1.1513631317077201E-4</v>
       </c>
-      <c r="Y105" s="73">
+      <c r="Y105" s="71">
         <v>1.23360335540113E-5</v>
       </c>
     </row>
@@ -49493,10 +49855,10 @@
       <c r="W106">
         <v>1.02800279616761E-4</v>
       </c>
-      <c r="X106" s="73">
+      <c r="X106" s="71">
         <v>2.8784078292693002E-5</v>
       </c>
-      <c r="Y106" s="73">
+      <c r="Y106" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -49573,7 +49935,7 @@
       <c r="X107">
         <v>1.1513631317077201E-4</v>
       </c>
-      <c r="Y107" s="73">
+      <c r="Y107" s="71">
         <v>4.5232123031374602E-5</v>
       </c>
     </row>
@@ -49647,10 +50009,10 @@
       <c r="W108">
         <v>1.48032402648135E-4</v>
       </c>
-      <c r="X108" s="73">
+      <c r="X108" s="71">
         <v>3.2896089477363403E-5</v>
       </c>
-      <c r="Y108" s="73">
+      <c r="Y108" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -49721,10 +50083,10 @@
       <c r="V109">
         <v>1.02800279616761E-3</v>
       </c>
-      <c r="W109" s="73">
+      <c r="W109" s="71">
         <v>6.9904190139397201E-5</v>
       </c>
-      <c r="X109" s="73">
+      <c r="X109" s="71">
         <v>1.23360335540113E-5</v>
       </c>
       <c r="Y109">
@@ -49798,10 +50160,10 @@
       <c r="V110">
         <v>1.11024301986101E-4</v>
       </c>
-      <c r="W110" s="73">
+      <c r="W110" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
-      <c r="X110" s="73">
+      <c r="X110" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
       <c r="Y110">
@@ -49878,10 +50240,10 @@
       <c r="W111">
         <v>2.34384637526214E-4</v>
       </c>
-      <c r="X111" s="73">
+      <c r="X111" s="71">
         <v>4.9344134216045098E-5</v>
       </c>
-      <c r="Y111" s="73">
+      <c r="Y111" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -49955,10 +50317,10 @@
       <c r="W112">
         <v>1.7681648094082801E-4</v>
       </c>
-      <c r="X112" s="73">
+      <c r="X112" s="71">
         <v>2.8784078292693002E-5</v>
       </c>
-      <c r="Y112" s="73">
+      <c r="Y112" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -50032,10 +50394,10 @@
       <c r="W113">
         <v>2.2204860397220301E-4</v>
       </c>
-      <c r="X113" s="73">
+      <c r="X113" s="71">
         <v>3.7008100662033798E-5</v>
       </c>
-      <c r="Y113" s="73">
+      <c r="Y113" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -50112,7 +50474,7 @@
       <c r="X114">
         <v>1.48032402648135E-4</v>
       </c>
-      <c r="Y114" s="73">
+      <c r="Y114" s="71">
         <v>1.6448044738681702E-5</v>
       </c>
     </row>
@@ -50183,13 +50545,13 @@
       <c r="V115">
         <v>9.1697849418150403E-4</v>
       </c>
-      <c r="W115" s="73">
+      <c r="W115" s="71">
         <v>8.6352234878078903E-5</v>
       </c>
-      <c r="X115" s="73">
+      <c r="X115" s="71">
         <v>1.23360335540113E-5</v>
       </c>
-      <c r="Y115" s="73">
+      <c r="Y115" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -50263,10 +50625,10 @@
       <c r="W116">
         <v>1.5625642501747601E-4</v>
       </c>
-      <c r="X116" s="73">
+      <c r="X116" s="71">
         <v>2.4672067108022502E-5</v>
       </c>
-      <c r="Y116" s="73">
+      <c r="Y116" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -50343,7 +50705,7 @@
       <c r="X117">
         <v>1.11024301986101E-4</v>
       </c>
-      <c r="Y117" s="73">
+      <c r="Y117" s="71">
         <v>1.23360335540113E-5</v>
       </c>
     </row>
@@ -50420,7 +50782,7 @@
       <c r="X118">
         <v>1.72704469756158E-4</v>
       </c>
-      <c r="Y118" s="73">
+      <c r="Y118" s="71">
         <v>1.23360335540113E-5</v>
       </c>
     </row>
@@ -50494,10 +50856,10 @@
       <c r="W119">
         <v>2.4260865989555501E-4</v>
       </c>
-      <c r="X119" s="73">
+      <c r="X119" s="71">
         <v>2.8784078292693002E-5</v>
       </c>
-      <c r="Y119" s="73">
+      <c r="Y119" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -50571,10 +50933,10 @@
       <c r="W120">
         <v>2.4260865989555501E-4</v>
       </c>
-      <c r="X120" s="73">
+      <c r="X120" s="71">
         <v>4.11201118467042E-5</v>
       </c>
-      <c r="Y120" s="73">
+      <c r="Y120" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -50651,7 +51013,7 @@
       <c r="X121">
         <v>1.68592458571487E-4</v>
       </c>
-      <c r="Y121" s="73">
+      <c r="Y121" s="71">
         <v>1.23360335540113E-5</v>
       </c>
     </row>
@@ -50728,7 +51090,7 @@
       <c r="X122">
         <v>1.06912290801431E-4</v>
       </c>
-      <c r="Y122" s="73">
+      <c r="Y122" s="71">
         <v>1.23360335540113E-5</v>
       </c>
     </row>
@@ -50802,7 +51164,7 @@
       <c r="W123">
         <v>4.9344134216045097E-4</v>
       </c>
-      <c r="X123" s="73">
+      <c r="X123" s="71">
         <v>6.5792178954726806E-5</v>
       </c>
       <c r="Y123">
@@ -50879,10 +51241,10 @@
       <c r="W124">
         <v>2.01488548048851E-4</v>
       </c>
-      <c r="X124" s="73">
+      <c r="X124" s="71">
         <v>6.5792178954726806E-5</v>
       </c>
-      <c r="Y124" s="73">
+      <c r="Y124" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -50959,7 +51321,7 @@
       <c r="X125">
         <v>1.2336033554011301E-4</v>
       </c>
-      <c r="Y125" s="73">
+      <c r="Y125" s="71">
         <v>1.23360335540113E-5</v>
       </c>
     </row>
@@ -51033,10 +51395,10 @@
       <c r="W126">
         <v>4.1942514083638299E-4</v>
       </c>
-      <c r="X126" s="73">
+      <c r="X126" s="71">
         <v>8.6352234878078903E-5</v>
       </c>
-      <c r="Y126" s="73">
+      <c r="Y126" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -51110,10 +51472,10 @@
       <c r="W127">
         <v>3.6596899543566802E-4</v>
       </c>
-      <c r="X127" s="73">
+      <c r="X127" s="71">
         <v>6.9904190139397201E-5</v>
       </c>
-      <c r="Y127" s="73">
+      <c r="Y127" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -51190,7 +51552,7 @@
       <c r="X128">
         <v>1.72704469756158E-4</v>
       </c>
-      <c r="Y128" s="73">
+      <c r="Y128" s="71">
         <v>2.4672067108022502E-5</v>
       </c>
     </row>
@@ -51264,10 +51626,10 @@
       <c r="W129">
         <v>2.5083268226489599E-4</v>
       </c>
-      <c r="X129" s="73">
+      <c r="X129" s="71">
         <v>4.5232123031374602E-5</v>
       </c>
-      <c r="Y129" s="73">
+      <c r="Y129" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -51341,10 +51703,10 @@
       <c r="W130">
         <v>2.46720671080225E-4</v>
       </c>
-      <c r="X130" s="73">
+      <c r="X130" s="71">
         <v>6.5792178954726806E-5</v>
       </c>
-      <c r="Y130" s="73">
+      <c r="Y130" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -51418,10 +51780,10 @@
       <c r="W131">
         <v>2.2204860397220301E-4</v>
       </c>
-      <c r="X131" s="73">
+      <c r="X131" s="71">
         <v>3.7008100662033798E-5</v>
       </c>
-      <c r="Y131" s="73">
+      <c r="Y131" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -51498,7 +51860,7 @@
       <c r="X132">
         <v>2.0560055923352099E-4</v>
       </c>
-      <c r="Y132" s="73">
+      <c r="Y132" s="71">
         <v>2.05600559233521E-5</v>
       </c>
     </row>
@@ -51572,10 +51934,10 @@
       <c r="W133">
         <v>4.1531312965171298E-4</v>
       </c>
-      <c r="X133" s="73">
+      <c r="X133" s="71">
         <v>9.0464246062749298E-5</v>
       </c>
-      <c r="Y133" s="73">
+      <c r="Y133" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -51649,10 +52011,10 @@
       <c r="W134">
         <v>2.0971257041819201E-4</v>
       </c>
-      <c r="X134" s="73">
+      <c r="X134" s="71">
         <v>2.8784078292693002E-5</v>
       </c>
-      <c r="Y134" s="73">
+      <c r="Y134" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -51729,7 +52091,7 @@
       <c r="X135">
         <v>1.1513631317077201E-4</v>
       </c>
-      <c r="Y135" s="73">
+      <c r="Y135" s="71">
         <v>1.6448044738681702E-5</v>
       </c>
     </row>
@@ -51803,10 +52165,10 @@
       <c r="W136">
         <v>2.1793659278753199E-4</v>
       </c>
-      <c r="X136" s="73">
+      <c r="X136" s="71">
         <v>9.0464246062749298E-5</v>
       </c>
-      <c r="Y136" s="73">
+      <c r="Y136" s="71">
         <v>2.8784078292693002E-5</v>
       </c>
     </row>
@@ -51883,7 +52245,7 @@
       <c r="X137">
         <v>1.9737653686418001E-4</v>
       </c>
-      <c r="Y137" s="73">
+      <c r="Y137" s="71">
         <v>9.4576257247419706E-5</v>
       </c>
     </row>
@@ -51957,10 +52319,10 @@
       <c r="W138">
         <v>2.7550474937291798E-4</v>
       </c>
-      <c r="X138" s="73">
+      <c r="X138" s="71">
         <v>6.5792178954726806E-5</v>
       </c>
-      <c r="Y138" s="73">
+      <c r="Y138" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -52034,10 +52396,10 @@
       <c r="W139">
         <v>2.2616061515687299E-4</v>
       </c>
-      <c r="X139" s="73">
+      <c r="X139" s="71">
         <v>4.11201118467042E-5</v>
       </c>
-      <c r="Y139" s="73">
+      <c r="Y139" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -52108,7 +52470,7 @@
       <c r="V140">
         <v>4.27649163205724E-4</v>
       </c>
-      <c r="W140" s="73">
+      <c r="W140" s="71">
         <v>3.2896089477363403E-5</v>
       </c>
       <c r="X140">
@@ -52188,10 +52550,10 @@
       <c r="W141">
         <v>3.6185698425099697E-4</v>
       </c>
-      <c r="X141" s="73">
+      <c r="X141" s="71">
         <v>6.1680167770056303E-5</v>
       </c>
-      <c r="Y141" s="73">
+      <c r="Y141" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -52268,7 +52630,7 @@
       <c r="X142">
         <v>3.2896089477363398E-4</v>
       </c>
-      <c r="Y142" s="73">
+      <c r="Y142" s="71">
         <v>4.9344134216045098E-5</v>
       </c>
     </row>
@@ -52345,7 +52707,7 @@
       <c r="X143">
         <v>4.3176117439039401E-4</v>
       </c>
-      <c r="Y143" s="73">
+      <c r="Y143" s="71">
         <v>6.5792178954726806E-5</v>
       </c>
     </row>
@@ -52422,7 +52784,7 @@
       <c r="X144">
         <v>2.7550474937291798E-4</v>
       </c>
-      <c r="Y144" s="73">
+      <c r="Y144" s="71">
         <v>2.8784078292693002E-5</v>
       </c>
     </row>
@@ -52496,10 +52858,10 @@
       <c r="W145">
         <v>1.1924832435544199E-4</v>
       </c>
-      <c r="X145" s="73">
+      <c r="X145" s="71">
         <v>3.7008100662033798E-5</v>
       </c>
-      <c r="Y145" s="73">
+      <c r="Y145" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -52576,7 +52938,7 @@
       <c r="X146">
         <v>2.7961676055758902E-4</v>
       </c>
-      <c r="Y146" s="73">
+      <c r="Y146" s="71">
         <v>2.4672067108022502E-5</v>
       </c>
     </row>
@@ -52653,7 +53015,7 @@
       <c r="X147">
         <v>5.6334553229984801E-4</v>
       </c>
-      <c r="Y147" s="73">
+      <c r="Y147" s="71">
         <v>6.5792178954726806E-5</v>
       </c>
     </row>
@@ -52724,13 +53086,13 @@
       <c r="V148">
         <v>9.5809860602820798E-4</v>
       </c>
-      <c r="W148" s="73">
+      <c r="W148" s="71">
         <v>4.5232123031374602E-5</v>
       </c>
-      <c r="X148" s="73">
+      <c r="X148" s="71">
         <v>1.23360335540113E-5</v>
       </c>
-      <c r="Y148" s="73">
+      <c r="Y148" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -52804,10 +53166,10 @@
       <c r="W149">
         <v>3.3307290595830399E-4</v>
       </c>
-      <c r="X149" s="73">
+      <c r="X149" s="71">
         <v>6.1680167770056303E-5</v>
       </c>
-      <c r="Y149" s="73">
+      <c r="Y149" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -52884,7 +53246,7 @@
       <c r="X150">
         <v>2.7961676055758902E-4</v>
       </c>
-      <c r="Y150" s="73">
+      <c r="Y150" s="71">
         <v>4.5232123031374602E-5</v>
       </c>
     </row>
@@ -52961,7 +53323,7 @@
       <c r="X151">
         <v>5.6745754348451797E-4</v>
       </c>
-      <c r="Y151" s="73">
+      <c r="Y151" s="71">
         <v>7.8128212508738005E-5</v>
       </c>
     </row>
@@ -53035,10 +53397,10 @@
       <c r="W152">
         <v>3.6596899543566802E-4</v>
       </c>
-      <c r="X152" s="73">
+      <c r="X152" s="71">
         <v>9.0464246062749298E-5</v>
       </c>
-      <c r="Y152" s="73">
+      <c r="Y152" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -53115,7 +53477,7 @@
       <c r="X153">
         <v>1.1924832435544199E-4</v>
       </c>
-      <c r="Y153" s="73">
+      <c r="Y153" s="71">
         <v>1.23360335540113E-5</v>
       </c>
     </row>
@@ -53189,10 +53551,10 @@
       <c r="W154">
         <v>3.74193017805008E-4</v>
       </c>
-      <c r="X154" s="73">
+      <c r="X154" s="71">
         <v>8.22402236934084E-5</v>
       </c>
-      <c r="Y154" s="73">
+      <c r="Y154" s="71">
         <v>1.23360335540113E-5</v>
       </c>
     </row>
@@ -53266,7 +53628,7 @@
       <c r="W155">
         <v>1.80928492125499E-4</v>
       </c>
-      <c r="X155" s="73">
+      <c r="X155" s="71">
         <v>4.5232123031374602E-5</v>
       </c>
       <c r="Y155">
@@ -53346,7 +53708,7 @@
       <c r="X156">
         <v>1.5625642501747601E-4</v>
       </c>
-      <c r="Y156" s="73">
+      <c r="Y156" s="71">
         <v>1.23360335540113E-5</v>
       </c>
     </row>
@@ -53423,7 +53785,7 @@
       <c r="X157">
         <v>3.2896089477363398E-4</v>
       </c>
-      <c r="Y157" s="73">
+      <c r="Y157" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -53497,10 +53859,10 @@
       <c r="W158">
         <v>3.9064106254369001E-4</v>
       </c>
-      <c r="X158" s="73">
+      <c r="X158" s="71">
         <v>6.9904190139397201E-5</v>
       </c>
-      <c r="Y158" s="73">
+      <c r="Y158" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -53577,7 +53939,7 @@
       <c r="X159">
         <v>1.48032402648135E-4</v>
       </c>
-      <c r="Y159" s="73">
+      <c r="Y159" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -53648,13 +54010,13 @@
       <c r="V160">
         <v>4.1120111846704198E-4</v>
       </c>
-      <c r="W160" s="73">
+      <c r="W160" s="71">
         <v>3.2896089477363403E-5</v>
       </c>
-      <c r="X160" s="73">
+      <c r="X160" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
-      <c r="Y160" s="73">
+      <c r="Y160" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -53728,10 +54090,10 @@
       <c r="W161">
         <v>1.3569636909412401E-4</v>
       </c>
-      <c r="X161" s="73">
+      <c r="X161" s="71">
         <v>2.4672067108022502E-5</v>
       </c>
-      <c r="Y161" s="73">
+      <c r="Y161" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -53808,7 +54170,7 @@
       <c r="X162">
         <v>2.7550474937291798E-4</v>
       </c>
-      <c r="Y162" s="73">
+      <c r="Y162" s="71">
         <v>3.2896089477363403E-5</v>
       </c>
     </row>
@@ -53882,10 +54244,10 @@
       <c r="W163">
         <v>2.9195279411159999E-4</v>
       </c>
-      <c r="X163" s="73">
+      <c r="X163" s="71">
         <v>8.6352234878078903E-5</v>
       </c>
-      <c r="Y163" s="73">
+      <c r="Y163" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -53962,7 +54324,7 @@
       <c r="X164">
         <v>2.8784078292692997E-4</v>
       </c>
-      <c r="Y164" s="73">
+      <c r="Y164" s="71">
         <v>8.6352234878078903E-5</v>
       </c>
     </row>
@@ -54036,10 +54398,10 @@
       <c r="W165">
         <v>2.13824581602862E-4</v>
       </c>
-      <c r="X165" s="73">
+      <c r="X165" s="71">
         <v>4.5232123031374602E-5</v>
       </c>
-      <c r="Y165" s="73">
+      <c r="Y165" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -54116,7 +54478,7 @@
       <c r="X166">
         <v>2.13824581602862E-4</v>
       </c>
-      <c r="Y166" s="73">
+      <c r="Y166" s="71">
         <v>2.4672067108022502E-5</v>
       </c>
     </row>
@@ -54190,10 +54552,10 @@
       <c r="W167">
         <v>5.09889386899132E-4</v>
       </c>
-      <c r="X167" s="73">
+      <c r="X167" s="71">
         <v>5.7568156585385901E-5</v>
       </c>
-      <c r="Y167" s="73">
+      <c r="Y167" s="71">
         <v>1.6448044738681702E-5</v>
       </c>
     </row>
@@ -54264,13 +54626,13 @@
       <c r="V168">
         <v>1.3158435790945399E-4</v>
       </c>
-      <c r="W168" s="73">
+      <c r="W168" s="71">
         <v>4.9344134216045098E-5</v>
       </c>
-      <c r="X168" s="73">
+      <c r="X168" s="71">
         <v>2.05600559233521E-5</v>
       </c>
-      <c r="Y168" s="73">
+      <c r="Y168" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -54344,10 +54706,10 @@
       <c r="W169">
         <v>2.46720671080225E-4</v>
       </c>
-      <c r="X169" s="73">
+      <c r="X169" s="71">
         <v>2.4672067108022502E-5</v>
       </c>
-      <c r="Y169" s="73">
+      <c r="Y169" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -54501,7 +54863,7 @@
       <c r="X171">
         <v>2.9606480529627001E-4</v>
       </c>
-      <c r="Y171" s="73">
+      <c r="Y171" s="71">
         <v>7.8128212508738005E-5</v>
       </c>
     </row>
@@ -54578,7 +54940,7 @@
       <c r="X172">
         <v>1.02800279616761E-4</v>
       </c>
-      <c r="Y172" s="73">
+      <c r="Y172" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -54655,7 +55017,7 @@
       <c r="X173">
         <v>1.1513631317077201E-4</v>
       </c>
-      <c r="Y173" s="73">
+      <c r="Y173" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -54732,7 +55094,7 @@
       <c r="X174">
         <v>1.02800279616761E-4</v>
       </c>
-      <c r="Y174" s="73">
+      <c r="Y174" s="71">
         <v>1.23360335540113E-5</v>
       </c>
     </row>
@@ -54806,7 +55168,7 @@
       <c r="W175">
         <v>1.9326452567951E-4</v>
       </c>
-      <c r="X175" s="73">
+      <c r="X175" s="71">
         <v>4.9344134216045098E-5</v>
       </c>
       <c r="Y175">
@@ -54886,7 +55248,7 @@
       <c r="X176">
         <v>1.80928492125499E-4</v>
       </c>
-      <c r="Y176" s="73">
+      <c r="Y176" s="71">
         <v>1.6448044738681702E-5</v>
       </c>
     </row>
@@ -54963,7 +55325,7 @@
       <c r="X177">
         <v>4.4820921912907597E-4</v>
       </c>
-      <c r="Y177" s="73">
+      <c r="Y177" s="71">
         <v>2.05600559233521E-5</v>
       </c>
     </row>
@@ -55037,10 +55399,10 @@
       <c r="W178">
         <v>4.4820921912907597E-4</v>
       </c>
-      <c r="X178" s="73">
+      <c r="X178" s="71">
         <v>9.8688268432090101E-5</v>
       </c>
-      <c r="Y178" s="73">
+      <c r="Y178" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -55117,7 +55479,7 @@
       <c r="X179">
         <v>1.6448044738681699E-4</v>
       </c>
-      <c r="Y179" s="73">
+      <c r="Y179" s="71">
         <v>1.23360335540113E-5</v>
       </c>
     </row>
@@ -55188,13 +55550,13 @@
       <c r="V180">
         <v>3.7008100662033798E-4</v>
       </c>
-      <c r="W180" s="73">
+      <c r="W180" s="71">
         <v>4.11201118467042E-5</v>
       </c>
-      <c r="X180" s="73">
+      <c r="X180" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
-      <c r="Y180" s="73">
+      <c r="Y180" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -55268,10 +55630,10 @@
       <c r="W181">
         <v>1.1924832435544199E-4</v>
       </c>
-      <c r="X181" s="73">
+      <c r="X181" s="71">
         <v>1.6448044738681702E-5</v>
       </c>
-      <c r="Y181" s="73">
+      <c r="Y181" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -55348,7 +55710,7 @@
       <c r="X182">
         <v>3.41296928327645E-4</v>
       </c>
-      <c r="Y182" s="73">
+      <c r="Y182" s="71">
         <v>4.5232123031374602E-5</v>
       </c>
     </row>
@@ -55422,10 +55784,10 @@
       <c r="W183">
         <v>3.82417040174349E-4</v>
       </c>
-      <c r="X183" s="73">
+      <c r="X183" s="71">
         <v>9.0464246062749298E-5</v>
       </c>
-      <c r="Y183" s="73">
+      <c r="Y183" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -55502,7 +55864,7 @@
       <c r="X184">
         <v>3.4952095069698601E-4</v>
       </c>
-      <c r="Y184" s="73">
+      <c r="Y184" s="71">
         <v>9.8688268432090101E-5</v>
       </c>
     </row>
@@ -55576,10 +55938,10 @@
       <c r="W185">
         <v>1.9737653686418001E-4</v>
       </c>
-      <c r="X185" s="73">
+      <c r="X185" s="71">
         <v>5.34561454007155E-5</v>
       </c>
-      <c r="Y185" s="73">
+      <c r="Y185" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -55656,7 +56018,7 @@
       <c r="X186">
         <v>2.8784078292692997E-4</v>
       </c>
-      <c r="Y186" s="73">
+      <c r="Y186" s="71">
         <v>2.8784078292693002E-5</v>
       </c>
     </row>
@@ -55730,10 +56092,10 @@
       <c r="W187">
         <v>7.0726592376331302E-4</v>
       </c>
-      <c r="X187" s="73">
+      <c r="X187" s="71">
         <v>6.1680167770056303E-5</v>
       </c>
-      <c r="Y187" s="73">
+      <c r="Y187" s="71">
         <v>1.6448044738681702E-5</v>
       </c>
     </row>
@@ -55804,13 +56166,13 @@
       <c r="V188">
         <v>1.6448044738681699E-4</v>
       </c>
-      <c r="W188" s="73">
+      <c r="W188" s="71">
         <v>4.9344134216045098E-5</v>
       </c>
-      <c r="X188" s="73">
+      <c r="X188" s="71">
         <v>2.8784078292693002E-5</v>
       </c>
-      <c r="Y188" s="73">
+      <c r="Y188" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -55884,10 +56246,10 @@
       <c r="W189">
         <v>2.4260865989555501E-4</v>
       </c>
-      <c r="X189" s="73">
+      <c r="X189" s="71">
         <v>3.2896089477363403E-5</v>
       </c>
-      <c r="Y189" s="73">
+      <c r="Y189" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -56041,7 +56403,7 @@
       <c r="X191">
         <v>3.08400838850282E-4</v>
       </c>
-      <c r="Y191" s="73">
+      <c r="Y191" s="71">
         <v>8.6352234878078903E-5</v>
       </c>
     </row>
@@ -56115,10 +56477,10 @@
       <c r="W192">
         <v>2.7139273818824802E-4</v>
       </c>
-      <c r="X192" s="73">
+      <c r="X192" s="71">
         <v>2.4672067108022502E-5</v>
       </c>
-      <c r="Y192" s="73">
+      <c r="Y192" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -56192,10 +56554,10 @@
       <c r="W193">
         <v>3.3307290595830399E-4</v>
       </c>
-      <c r="X193" s="73">
+      <c r="X193" s="71">
         <v>5.7568156585385901E-5</v>
       </c>
-      <c r="Y193" s="73">
+      <c r="Y193" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -56272,7 +56634,7 @@
       <c r="X194">
         <v>1.68592458571487E-4</v>
       </c>
-      <c r="Y194" s="73">
+      <c r="Y194" s="71">
         <v>1.23360335540113E-5</v>
       </c>
     </row>
@@ -56343,13 +56705,13 @@
       <c r="V195">
         <v>1.2048192771084299E-3</v>
       </c>
-      <c r="W195" s="73">
+      <c r="W195" s="71">
         <v>9.8688268432090101E-5</v>
       </c>
-      <c r="X195" s="73">
+      <c r="X195" s="71">
         <v>2.05600559233521E-5</v>
       </c>
-      <c r="Y195" s="73">
+      <c r="Y195" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -56423,10 +56785,10 @@
       <c r="W196">
         <v>2.4260865989555501E-4</v>
       </c>
-      <c r="X196" s="73">
+      <c r="X196" s="71">
         <v>2.8784078292693002E-5</v>
       </c>
-      <c r="Y196" s="73">
+      <c r="Y196" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -56503,7 +56865,7 @@
       <c r="X197">
         <v>1.3569636909412401E-4</v>
       </c>
-      <c r="Y197" s="73">
+      <c r="Y197" s="71">
         <v>1.23360335540113E-5</v>
       </c>
     </row>
@@ -56580,7 +56942,7 @@
       <c r="X198">
         <v>2.0971257041819201E-4</v>
       </c>
-      <c r="Y198" s="73">
+      <c r="Y198" s="71">
         <v>1.23360335540113E-5</v>
       </c>
     </row>
@@ -56654,10 +57016,10 @@
       <c r="W199">
         <v>2.7550474937291798E-4</v>
       </c>
-      <c r="X199" s="73">
+      <c r="X199" s="71">
         <v>5.7568156585385901E-5</v>
       </c>
-      <c r="Y199" s="73">
+      <c r="Y199" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -56731,10 +57093,10 @@
       <c r="W200">
         <v>2.7961676055758902E-4</v>
       </c>
-      <c r="X200" s="73">
+      <c r="X200" s="71">
         <v>4.9344134216045098E-5</v>
       </c>
-      <c r="Y200" s="73">
+      <c r="Y200" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -56811,7 +57173,7 @@
       <c r="X201">
         <v>1.9737653686418001E-4</v>
       </c>
-      <c r="Y201" s="73">
+      <c r="Y201" s="71">
         <v>1.23360335540113E-5</v>
       </c>
     </row>
@@ -56888,7 +57250,7 @@
       <c r="X202">
         <v>1.4392039146346499E-4</v>
       </c>
-      <c r="Y202" s="73">
+      <c r="Y202" s="71">
         <v>1.23360335540113E-5</v>
       </c>
     </row>
@@ -56962,10 +57324,10 @@
       <c r="W203">
         <v>6.9081787902463101E-4</v>
       </c>
-      <c r="X203" s="73">
+      <c r="X203" s="71">
         <v>8.6352234878078903E-5</v>
       </c>
-      <c r="Y203" s="73">
+      <c r="Y203" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -57039,10 +57401,10 @@
       <c r="W204">
         <v>2.5083268226489599E-4</v>
       </c>
-      <c r="X204" s="73">
+      <c r="X204" s="71">
         <v>5.7568156585385901E-5</v>
       </c>
-      <c r="Y204" s="73">
+      <c r="Y204" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -57119,7 +57481,7 @@
       <c r="X205">
         <v>1.3569636909412401E-4</v>
       </c>
-      <c r="Y205" s="73">
+      <c r="Y205" s="71">
         <v>1.6448044738681702E-5</v>
       </c>
     </row>
@@ -57193,10 +57555,10 @@
       <c r="W206">
         <v>4.4820921912907597E-4</v>
       </c>
-      <c r="X206" s="73">
+      <c r="X206" s="71">
         <v>9.8688268432090101E-5</v>
       </c>
-      <c r="Y206" s="73">
+      <c r="Y206" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -57273,7 +57635,7 @@
       <c r="X207">
         <v>1.11024301986101E-4</v>
       </c>
-      <c r="Y207" s="73">
+      <c r="Y207" s="71">
         <v>1.23360335540113E-5</v>
       </c>
     </row>
@@ -57350,7 +57712,7 @@
       <c r="X208">
         <v>2.1793659278753199E-4</v>
       </c>
-      <c r="Y208" s="73">
+      <c r="Y208" s="71">
         <v>2.05600559233521E-5</v>
       </c>
     </row>
@@ -57424,10 +57786,10 @@
       <c r="W209">
         <v>3.2896089477363398E-4</v>
       </c>
-      <c r="X209" s="73">
+      <c r="X209" s="71">
         <v>6.9904190139397201E-5</v>
       </c>
-      <c r="Y209" s="73">
+      <c r="Y209" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -57501,10 +57863,10 @@
       <c r="W210">
         <v>3.2073687240429303E-4</v>
       </c>
-      <c r="X210" s="73">
+      <c r="X210" s="71">
         <v>7.4016201324067596E-5</v>
       </c>
-      <c r="Y210" s="73">
+      <c r="Y210" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -57578,10 +57940,10 @@
       <c r="W211">
         <v>2.7961676055758902E-4</v>
       </c>
-      <c r="X211" s="73">
+      <c r="X211" s="71">
         <v>6.1680167770056303E-5</v>
       </c>
-      <c r="Y211" s="73">
+      <c r="Y211" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -57658,7 +58020,7 @@
       <c r="X212">
         <v>2.1793659278753199E-4</v>
       </c>
-      <c r="Y212" s="73">
+      <c r="Y212" s="71">
         <v>1.23360335540113E-5</v>
       </c>
     </row>
@@ -57735,7 +58097,7 @@
       <c r="X213">
         <v>1.1924832435544199E-4</v>
       </c>
-      <c r="Y213" s="73">
+      <c r="Y213" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -57809,10 +58171,10 @@
       <c r="W214">
         <v>2.5083268226489599E-4</v>
       </c>
-      <c r="X214" s="73">
+      <c r="X214" s="71">
         <v>4.11201118467042E-5</v>
       </c>
-      <c r="Y214" s="73">
+      <c r="Y214" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -57889,7 +58251,7 @@
       <c r="X215">
         <v>2.4260865989555501E-4</v>
       </c>
-      <c r="Y215" s="73">
+      <c r="Y215" s="71">
         <v>2.8784078292693002E-5</v>
       </c>
     </row>
@@ -57966,7 +58328,7 @@
       <c r="X216">
         <v>1.02800279616761E-4</v>
       </c>
-      <c r="Y216" s="73">
+      <c r="Y216" s="71">
         <v>3.7008100662033798E-5</v>
       </c>
     </row>
@@ -58117,10 +58479,10 @@
       <c r="W218">
         <v>3.7008100662033798E-4</v>
       </c>
-      <c r="X218" s="73">
+      <c r="X218" s="71">
         <v>7.8128212508738005E-5</v>
       </c>
-      <c r="Y218" s="73">
+      <c r="Y218" s="71">
         <v>1.23360335540113E-5</v>
       </c>
     </row>
@@ -58194,10 +58556,10 @@
       <c r="W219">
         <v>3.7008100662033798E-4</v>
       </c>
-      <c r="X219" s="73">
+      <c r="X219" s="71">
         <v>6.9904190139397201E-5</v>
       </c>
-      <c r="Y219" s="73">
+      <c r="Y219" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -58268,10 +58630,10 @@
       <c r="V220">
         <v>4.9755335334512104E-4</v>
       </c>
-      <c r="W220" s="73">
+      <c r="W220" s="71">
         <v>4.5232123031374602E-5</v>
       </c>
-      <c r="X220" s="73">
+      <c r="X220" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
       <c r="Y220">
@@ -58348,10 +58710,10 @@
       <c r="W221">
         <v>5.1400139808380305E-4</v>
       </c>
-      <c r="X221" s="73">
+      <c r="X221" s="71">
         <v>8.6352234878078903E-5</v>
       </c>
-      <c r="Y221" s="73">
+      <c r="Y221" s="71">
         <v>1.23360335540113E-5</v>
       </c>
     </row>
@@ -58425,10 +58787,10 @@
       <c r="W222">
         <v>2.5083268226489599E-4</v>
       </c>
-      <c r="X222" s="73">
+      <c r="X222" s="71">
         <v>3.2896089477363403E-5</v>
       </c>
-      <c r="Y222" s="73">
+      <c r="Y222" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -58502,10 +58864,10 @@
       <c r="W223">
         <v>3.1662486121962301E-4</v>
       </c>
-      <c r="X223" s="73">
+      <c r="X223" s="71">
         <v>6.1680167770056303E-5</v>
       </c>
-      <c r="Y223" s="73">
+      <c r="Y223" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -58582,7 +58944,7 @@
       <c r="X224">
         <v>1.39808380278794E-4</v>
       </c>
-      <c r="Y224" s="73">
+      <c r="Y224" s="71">
         <v>1.23360335540113E-5</v>
       </c>
     </row>
@@ -58656,7 +59018,7 @@
       <c r="W225">
         <v>1.06912290801431E-4</v>
       </c>
-      <c r="X225" s="73">
+      <c r="X225" s="71">
         <v>2.05600559233521E-5</v>
       </c>
       <c r="Y225">
@@ -58733,10 +59095,10 @@
       <c r="W226">
         <v>2.3027262634154401E-4</v>
       </c>
-      <c r="X226" s="73">
+      <c r="X226" s="71">
         <v>3.7008100662033798E-5</v>
       </c>
-      <c r="Y226" s="73">
+      <c r="Y226" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -58813,7 +59175,7 @@
       <c r="X227">
         <v>1.2336033554011301E-4</v>
       </c>
-      <c r="Y227" s="73">
+      <c r="Y227" s="71">
         <v>1.23360335540113E-5</v>
       </c>
     </row>
@@ -58890,7 +59252,7 @@
       <c r="X228">
         <v>1.8504050331016899E-4</v>
       </c>
-      <c r="Y228" s="73">
+      <c r="Y228" s="71">
         <v>1.23360335540113E-5</v>
       </c>
     </row>
@@ -58964,10 +59326,10 @@
       <c r="W229">
         <v>2.5905670463423699E-4</v>
       </c>
-      <c r="X229" s="73">
+      <c r="X229" s="71">
         <v>3.2896089477363403E-5</v>
       </c>
-      <c r="Y229" s="73">
+      <c r="Y229" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -59041,10 +59403,10 @@
       <c r="W230">
         <v>2.2204860397220301E-4</v>
       </c>
-      <c r="X230" s="73">
+      <c r="X230" s="71">
         <v>5.34561454007155E-5</v>
       </c>
-      <c r="Y230" s="73">
+      <c r="Y230" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -59121,7 +59483,7 @@
       <c r="X231">
         <v>2.0560055923352099E-4</v>
       </c>
-      <c r="Y231" s="73">
+      <c r="Y231" s="71">
         <v>1.23360335540113E-5</v>
       </c>
     </row>
@@ -59198,7 +59560,7 @@
       <c r="X232">
         <v>1.80928492125499E-4</v>
       </c>
-      <c r="Y232" s="73">
+      <c r="Y232" s="71">
         <v>1.23360335540113E-5</v>
       </c>
     </row>
@@ -59272,10 +59634,10 @@
       <c r="W233">
         <v>6.4147374480858605E-4</v>
       </c>
-      <c r="X233" s="73">
+      <c r="X233" s="71">
         <v>7.4016201324067596E-5</v>
       </c>
-      <c r="Y233" s="73">
+      <c r="Y233" s="71">
         <v>1.6448044738681702E-5</v>
       </c>
     </row>
@@ -59349,10 +59711,10 @@
       <c r="W234">
         <v>2.13824581602862E-4</v>
       </c>
-      <c r="X234" s="73">
+      <c r="X234" s="71">
         <v>6.5792178954726806E-5</v>
       </c>
-      <c r="Y234" s="73">
+      <c r="Y234" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -59429,7 +59791,7 @@
       <c r="X235">
         <v>1.4392039146346499E-4</v>
       </c>
-      <c r="Y235" s="73">
+      <c r="Y235" s="71">
         <v>1.23360335540113E-5</v>
       </c>
     </row>
@@ -59503,10 +59865,10 @@
       <c r="W236">
         <v>4.4820921912907597E-4</v>
       </c>
-      <c r="X236" s="73">
+      <c r="X236" s="71">
         <v>9.8688268432090101E-5</v>
       </c>
-      <c r="Y236" s="73">
+      <c r="Y236" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -59583,7 +59945,7 @@
       <c r="X237">
         <v>1.1513631317077201E-4</v>
       </c>
-      <c r="Y237" s="73">
+      <c r="Y237" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -59660,7 +60022,7 @@
       <c r="X238">
         <v>2.34384637526214E-4</v>
       </c>
-      <c r="Y238" s="73">
+      <c r="Y238" s="71">
         <v>2.4672067108022502E-5</v>
       </c>
     </row>
@@ -59734,10 +60096,10 @@
       <c r="W239">
         <v>2.7139273818824802E-4</v>
       </c>
-      <c r="X239" s="73">
+      <c r="X239" s="71">
         <v>6.5792178954726806E-5</v>
       </c>
-      <c r="Y239" s="73">
+      <c r="Y239" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -59811,10 +60173,10 @@
       <c r="W240">
         <v>2.9195279411159999E-4</v>
       </c>
-      <c r="X240" s="73">
+      <c r="X240" s="71">
         <v>6.1680167770056303E-5</v>
       </c>
-      <c r="Y240" s="73">
+      <c r="Y240" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -59888,10 +60250,10 @@
       <c r="W241">
         <v>2.7139273818824802E-4</v>
       </c>
-      <c r="X241" s="73">
+      <c r="X241" s="71">
         <v>6.5792178954726806E-5</v>
       </c>
-      <c r="Y241" s="73">
+      <c r="Y241" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -59968,7 +60330,7 @@
       <c r="X242">
         <v>1.9737653686418001E-4</v>
       </c>
-      <c r="Y242" s="73">
+      <c r="Y242" s="71">
         <v>1.6448044738681702E-5</v>
       </c>
     </row>
@@ -60045,7 +60407,7 @@
       <c r="X243">
         <v>1.1924832435544199E-4</v>
       </c>
-      <c r="Y243" s="73">
+      <c r="Y243" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -60119,10 +60481,10 @@
       <c r="W244">
         <v>2.5083268226489599E-4</v>
       </c>
-      <c r="X244" s="73">
+      <c r="X244" s="71">
         <v>3.2896089477363403E-5</v>
       </c>
-      <c r="Y244" s="73">
+      <c r="Y244" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -60199,7 +60561,7 @@
       <c r="X245">
         <v>2.1793659278753199E-4</v>
       </c>
-      <c r="Y245" s="73">
+      <c r="Y245" s="71">
         <v>2.05600559233521E-5</v>
       </c>
     </row>
@@ -60273,10 +60635,10 @@
       <c r="W246">
         <v>2.46720671080225E-4</v>
       </c>
-      <c r="X246" s="73">
+      <c r="X246" s="71">
         <v>9.8688268432090101E-5</v>
       </c>
-      <c r="Y246" s="73">
+      <c r="Y246" s="71">
         <v>3.2896089477363403E-5</v>
       </c>
     </row>
@@ -60427,10 +60789,10 @@
       <c r="W248">
         <v>3.74193017805008E-4</v>
       </c>
-      <c r="X248" s="73">
+      <c r="X248" s="71">
         <v>6.9904190139397201E-5</v>
       </c>
-      <c r="Y248" s="73">
+      <c r="Y248" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -60504,10 +60866,10 @@
       <c r="W249">
         <v>3.3718491714297498E-4</v>
       </c>
-      <c r="X249" s="73">
+      <c r="X249" s="71">
         <v>6.1680167770056303E-5</v>
       </c>
-      <c r="Y249" s="73">
+      <c r="Y249" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -60578,10 +60940,10 @@
       <c r="V250">
         <v>4.9344134216045097E-4</v>
       </c>
-      <c r="W250" s="73">
+      <c r="W250" s="71">
         <v>4.9344134216045098E-5</v>
       </c>
-      <c r="X250" s="73">
+      <c r="X250" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
       <c r="Y250">
@@ -60661,7 +61023,7 @@
       <c r="X251">
         <v>1.02800279616761E-4</v>
       </c>
-      <c r="Y251" s="73">
+      <c r="Y251" s="71">
         <v>1.23360335540113E-5</v>
       </c>
     </row>
@@ -60735,10 +61097,10 @@
       <c r="W252">
         <v>3.1662486121962301E-4</v>
       </c>
-      <c r="X252" s="73">
+      <c r="X252" s="71">
         <v>2.8784078292693002E-5</v>
       </c>
-      <c r="Y252" s="73">
+      <c r="Y252" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -60812,10 +61174,10 @@
       <c r="W253">
         <v>2.8372877174225898E-4</v>
       </c>
-      <c r="X253" s="73">
+      <c r="X253" s="71">
         <v>6.5792178954726806E-5</v>
       </c>
-      <c r="Y253" s="73">
+      <c r="Y253" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -60892,7 +61254,7 @@
       <c r="X254">
         <v>1.6448044738681699E-4</v>
       </c>
-      <c r="Y254" s="73">
+      <c r="Y254" s="71">
         <v>1.23360335540113E-5</v>
       </c>
     </row>
@@ -60966,10 +61328,10 @@
       <c r="W255">
         <v>1.06912290801431E-4</v>
       </c>
-      <c r="X255" s="73">
+      <c r="X255" s="71">
         <v>2.4672067108022502E-5</v>
       </c>
-      <c r="Y255" s="73">
+      <c r="Y255" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -61043,10 +61405,10 @@
       <c r="W256">
         <v>2.0560055923352099E-4</v>
       </c>
-      <c r="X256" s="73">
+      <c r="X256" s="71">
         <v>3.2896089477363403E-5</v>
       </c>
-      <c r="Y256" s="73">
+      <c r="Y256" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -61123,7 +61485,7 @@
       <c r="X257">
         <v>1.27472346724783E-4</v>
       </c>
-      <c r="Y257" s="73">
+      <c r="Y257" s="71">
         <v>1.23360335540113E-5</v>
       </c>
     </row>
@@ -61200,7 +61562,7 @@
       <c r="X258">
         <v>1.80928492125499E-4</v>
       </c>
-      <c r="Y258" s="73">
+      <c r="Y258" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -61274,10 +61636,10 @@
       <c r="W259">
         <v>2.6728072700357702E-4</v>
       </c>
-      <c r="X259" s="73">
+      <c r="X259" s="71">
         <v>5.34561454007155E-5</v>
       </c>
-      <c r="Y259" s="73">
+      <c r="Y259" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -61351,10 +61713,10 @@
       <c r="W260">
         <v>2.5905670463423699E-4</v>
       </c>
-      <c r="X260" s="73">
+      <c r="X260" s="71">
         <v>5.7568156585385901E-5</v>
       </c>
-      <c r="Y260" s="73">
+      <c r="Y260" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -61431,7 +61793,7 @@
       <c r="X261">
         <v>2.2204860397220301E-4</v>
       </c>
-      <c r="Y261" s="73">
+      <c r="Y261" s="71">
         <v>1.23360335540113E-5</v>
       </c>
     </row>
@@ -61508,7 +61870,7 @@
       <c r="X262">
         <v>1.8504050331016899E-4</v>
       </c>
-      <c r="Y262" s="73">
+      <c r="Y262" s="71">
         <v>1.23360335540113E-5</v>
       </c>
     </row>
@@ -61582,10 +61944,10 @@
       <c r="W263">
         <v>5.9624162177721095E-4</v>
       </c>
-      <c r="X263" s="73">
+      <c r="X263" s="71">
         <v>6.1680167770056303E-5</v>
       </c>
-      <c r="Y263" s="73">
+      <c r="Y263" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -61659,10 +62021,10 @@
       <c r="W264">
         <v>2.2616061515687299E-4</v>
       </c>
-      <c r="X264" s="73">
+      <c r="X264" s="71">
         <v>6.1680167770056303E-5</v>
       </c>
-      <c r="Y264" s="73">
+      <c r="Y264" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -61739,7 +62101,7 @@
       <c r="X265">
         <v>1.3158435790945399E-4</v>
       </c>
-      <c r="Y265" s="73">
+      <c r="Y265" s="71">
         <v>1.6448044738681702E-5</v>
       </c>
     </row>
@@ -61813,10 +62175,10 @@
       <c r="W266">
         <v>4.4409720794440601E-4</v>
       </c>
-      <c r="X266" s="73">
+      <c r="X266" s="71">
         <v>9.0464246062749298E-5</v>
       </c>
-      <c r="Y266" s="73">
+      <c r="Y266" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -61893,7 +62255,7 @@
       <c r="X267">
         <v>1.11024301986101E-4</v>
       </c>
-      <c r="Y267" s="73">
+      <c r="Y267" s="71">
         <v>1.6448044738681702E-5</v>
       </c>
     </row>
@@ -61970,7 +62332,7 @@
       <c r="X268">
         <v>2.46720671080225E-4</v>
       </c>
-      <c r="Y268" s="73">
+      <c r="Y268" s="71">
         <v>2.05600559233521E-5</v>
       </c>
     </row>
@@ -62044,10 +62406,10 @@
       <c r="W269">
         <v>3.4540893951231502E-4</v>
       </c>
-      <c r="X269" s="73">
+      <c r="X269" s="71">
         <v>7.4016201324067596E-5</v>
       </c>
-      <c r="Y269" s="73">
+      <c r="Y269" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -62121,10 +62483,10 @@
       <c r="W270">
         <v>2.8372877174225898E-4</v>
       </c>
-      <c r="X270" s="73">
+      <c r="X270" s="71">
         <v>7.4016201324067596E-5</v>
       </c>
-      <c r="Y270" s="73">
+      <c r="Y270" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -62198,10 +62560,10 @@
       <c r="W271">
         <v>2.9195279411159999E-4</v>
       </c>
-      <c r="X271" s="73">
+      <c r="X271" s="71">
         <v>5.34561454007155E-5</v>
       </c>
-      <c r="Y271" s="73">
+      <c r="Y271" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -62278,7 +62640,7 @@
       <c r="X272">
         <v>2.1793659278753199E-4</v>
       </c>
-      <c r="Y272" s="73">
+      <c r="Y272" s="71">
         <v>1.23360335540113E-5</v>
       </c>
     </row>
@@ -62355,7 +62717,7 @@
       <c r="X273">
         <v>1.2336033554011301E-4</v>
       </c>
-      <c r="Y273" s="73">
+      <c r="Y273" s="71">
         <v>1.23360335540113E-5</v>
       </c>
     </row>
@@ -62429,10 +62791,10 @@
       <c r="W274">
         <v>2.6728072700357702E-4</v>
       </c>
-      <c r="X274" s="73">
+      <c r="X274" s="71">
         <v>4.11201118467042E-5</v>
       </c>
-      <c r="Y274" s="73">
+      <c r="Y274" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -62509,7 +62871,7 @@
       <c r="X275">
         <v>2.2616061515687299E-4</v>
       </c>
-      <c r="Y275" s="73">
+      <c r="Y275" s="71">
         <v>2.8784078292693002E-5</v>
       </c>
     </row>
@@ -62586,7 +62948,7 @@
       <c r="X276">
         <v>1.11024301986101E-4</v>
       </c>
-      <c r="Y276" s="73">
+      <c r="Y276" s="71">
         <v>3.2896089477363403E-5</v>
       </c>
     </row>
@@ -62737,10 +63099,10 @@
       <c r="W278">
         <v>3.6185698425099697E-4</v>
       </c>
-      <c r="X278" s="73">
+      <c r="X278" s="71">
         <v>7.4016201324067596E-5</v>
       </c>
-      <c r="Y278" s="73">
+      <c r="Y278" s="71">
         <v>1.23360335540113E-5</v>
       </c>
     </row>
@@ -62814,10 +63176,10 @@
       <c r="W279">
         <v>3.08400838850282E-4</v>
       </c>
-      <c r="X279" s="73">
+      <c r="X279" s="71">
         <v>7.4016201324067596E-5</v>
       </c>
-      <c r="Y279" s="73">
+      <c r="Y279" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -62888,10 +63250,10 @@
       <c r="V280">
         <v>5.1400139808380305E-4</v>
       </c>
-      <c r="W280" s="73">
+      <c r="W280" s="71">
         <v>3.7008100662033798E-5</v>
       </c>
-      <c r="X280" s="73">
+      <c r="X280" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
       <c r="Y280">
@@ -62968,10 +63330,10 @@
       <c r="W281">
         <v>4.9755335334512104E-4</v>
       </c>
-      <c r="X281" s="73">
+      <c r="X281" s="71">
         <v>9.4576257247419706E-5</v>
       </c>
-      <c r="Y281" s="73">
+      <c r="Y281" s="71">
         <v>1.23360335540113E-5</v>
       </c>
     </row>
@@ -63048,7 +63410,7 @@
       <c r="X282">
         <v>4.4409720794440601E-4</v>
       </c>
-      <c r="Y282" s="73">
+      <c r="Y282" s="71">
         <v>6.9904190139397201E-5</v>
       </c>
     </row>
@@ -63125,7 +63487,7 @@
       <c r="X283">
         <v>7.3193799087133496E-4</v>
       </c>
-      <c r="Y283" s="73">
+      <c r="Y283" s="71">
         <v>9.8688268432090101E-5</v>
       </c>
     </row>
@@ -63202,7 +63564,7 @@
       <c r="X284">
         <v>4.0297709609770098E-4</v>
       </c>
-      <c r="Y284" s="73">
+      <c r="Y284" s="71">
         <v>5.7568156585385901E-5</v>
       </c>
     </row>
@@ -63276,10 +63638,10 @@
       <c r="W285">
         <v>1.06912290801431E-4</v>
       </c>
-      <c r="X285" s="73">
+      <c r="X285" s="71">
         <v>1.6448044738681702E-5</v>
       </c>
-      <c r="Y285" s="73">
+      <c r="Y285" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -63356,7 +63718,7 @@
       <c r="X286">
         <v>3.9886508491303102E-4</v>
       </c>
-      <c r="Y286" s="73">
+      <c r="Y286" s="71">
         <v>6.1680167770056303E-5</v>
       </c>
     </row>
@@ -63433,7 +63795,7 @@
       <c r="X287">
         <v>1.06912290801431E-3</v>
       </c>
-      <c r="Y287" s="73">
+      <c r="Y287" s="71">
         <v>9.4576257247419706E-5</v>
       </c>
     </row>
@@ -63510,7 +63872,7 @@
       <c r="X288">
         <v>1.02800279616761E-4</v>
       </c>
-      <c r="Y288" s="73">
+      <c r="Y288" s="71">
         <v>1.23360335540113E-5</v>
       </c>
     </row>
@@ -63587,7 +63949,7 @@
       <c r="X289">
         <v>3.1662486121962301E-4</v>
       </c>
-      <c r="Y289" s="73">
+      <c r="Y289" s="71">
         <v>4.11201118467042E-5</v>
       </c>
     </row>
@@ -63741,7 +64103,7 @@
       <c r="X291">
         <v>3.9886508491303102E-4</v>
       </c>
-      <c r="Y291" s="73">
+      <c r="Y291" s="71">
         <v>7.4016201324067596E-5</v>
       </c>
     </row>
@@ -63818,7 +64180,7 @@
       <c r="X292">
         <v>7.4427402442534603E-4</v>
       </c>
-      <c r="Y292" s="73">
+      <c r="Y292" s="71">
         <v>8.6352234878078903E-5</v>
       </c>
     </row>
@@ -63895,7 +64257,7 @@
       <c r="X293">
         <v>4.0297709609770098E-4</v>
       </c>
-      <c r="Y293" s="73">
+      <c r="Y293" s="71">
         <v>4.5232123031374602E-5</v>
       </c>
     </row>
@@ -63969,10 +64331,10 @@
       <c r="W294">
         <v>1.60368436202146E-4</v>
       </c>
-      <c r="X294" s="73">
+      <c r="X294" s="71">
         <v>2.8784078292693002E-5</v>
       </c>
-      <c r="Y294" s="73">
+      <c r="Y294" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -64049,7 +64411,7 @@
       <c r="X295">
         <v>3.74193017805008E-4</v>
       </c>
-      <c r="Y295" s="73">
+      <c r="Y295" s="71">
         <v>6.1680167770056303E-5</v>
       </c>
     </row>
@@ -64126,7 +64488,7 @@
       <c r="X296">
         <v>1.0362268185369499E-3</v>
       </c>
-      <c r="Y296" s="73">
+      <c r="Y296" s="71">
         <v>9.4576257247419706E-5</v>
       </c>
     </row>
@@ -64200,10 +64562,10 @@
       <c r="W297">
         <v>4.68769275052428E-4</v>
       </c>
-      <c r="X297" s="73">
+      <c r="X297" s="71">
         <v>9.8688268432090101E-5</v>
       </c>
-      <c r="Y297" s="73">
+      <c r="Y297" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -64280,7 +64642,7 @@
       <c r="X298">
         <v>2.7961676055758902E-4</v>
       </c>
-      <c r="Y298" s="73">
+      <c r="Y298" s="71">
         <v>4.5232123031374602E-5</v>
       </c>
     </row>
@@ -64434,7 +64796,7 @@
       <c r="X300">
         <v>1.60368436202146E-4</v>
       </c>
-      <c r="Y300" s="73">
+      <c r="Y300" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -64511,7 +64873,7 @@
       <c r="X301">
         <v>1.27472346724783E-4</v>
       </c>
-      <c r="Y301" s="73">
+      <c r="Y301" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -64588,7 +64950,7 @@
       <c r="X302">
         <v>1.80928492125499E-4</v>
       </c>
-      <c r="Y302" s="73">
+      <c r="Y302" s="71">
         <v>1.23360335540113E-5</v>
       </c>
     </row>
@@ -64662,7 +65024,7 @@
       <c r="W303">
         <v>3.5363296188165602E-4</v>
       </c>
-      <c r="X303" s="73">
+      <c r="X303" s="71">
         <v>9.4576257247419706E-5</v>
       </c>
       <c r="Y303">
@@ -64742,7 +65104,7 @@
       <c r="X304">
         <v>3.6185698425099697E-4</v>
       </c>
-      <c r="Y304" s="73">
+      <c r="Y304" s="71">
         <v>5.7568156585385901E-5</v>
       </c>
     </row>
@@ -64896,7 +65258,7 @@
       <c r="X306">
         <v>1.9737653686418001E-4</v>
       </c>
-      <c r="Y306" s="73">
+      <c r="Y306" s="71">
         <v>1.23360335540113E-5</v>
       </c>
     </row>
@@ -64973,7 +65335,7 @@
       <c r="X307">
         <v>2.6316871581890701E-4</v>
       </c>
-      <c r="Y307" s="73">
+      <c r="Y307" s="71">
         <v>2.4672067108022502E-5</v>
       </c>
     </row>
@@ -65044,13 +65406,13 @@
       <c r="V308">
         <v>2.0560055923352099E-4</v>
       </c>
-      <c r="W308" s="73">
+      <c r="W308" s="71">
         <v>1.23360335540113E-5</v>
       </c>
-      <c r="X308" s="73">
+      <c r="X308" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
-      <c r="Y308" s="73">
+      <c r="Y308" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -65124,10 +65486,10 @@
       <c r="W309">
         <v>2.0560055923352099E-4</v>
       </c>
-      <c r="X309" s="73">
+      <c r="X309" s="71">
         <v>2.4672067108022502E-5</v>
       </c>
-      <c r="Y309" s="73">
+      <c r="Y309" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -65355,10 +65717,10 @@
       <c r="W312">
         <v>3.9064106254369001E-4</v>
       </c>
-      <c r="X312" s="73">
+      <c r="X312" s="71">
         <v>8.22402236934084E-5</v>
       </c>
-      <c r="Y312" s="73">
+      <c r="Y312" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -65435,7 +65797,7 @@
       <c r="X313">
         <v>3.5774497306632701E-4</v>
       </c>
-      <c r="Y313" s="73">
+      <c r="Y313" s="71">
         <v>3.7008100662033798E-5</v>
       </c>
     </row>
@@ -65512,7 +65874,7 @@
       <c r="X314">
         <v>1.27472346724783E-4</v>
       </c>
-      <c r="Y314" s="73">
+      <c r="Y314" s="71">
         <v>2.05600559233521E-5</v>
       </c>
     </row>
@@ -65583,13 +65945,13 @@
       <c r="V315">
         <v>1.3158435790945399E-4</v>
       </c>
-      <c r="W315" s="73">
+      <c r="W315" s="71">
         <v>4.9344134216045098E-5</v>
       </c>
-      <c r="X315" s="73">
+      <c r="X315" s="71">
         <v>2.05600559233521E-5</v>
       </c>
-      <c r="Y315" s="73">
+      <c r="Y315" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -65663,10 +66025,10 @@
       <c r="W316">
         <v>4.1942514083638299E-4</v>
       </c>
-      <c r="X316" s="73">
+      <c r="X316" s="71">
         <v>7.4016201324067596E-5</v>
       </c>
-      <c r="Y316" s="73">
+      <c r="Y316" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -65897,7 +66259,7 @@
       <c r="X319">
         <v>1.7681648094082801E-4</v>
       </c>
-      <c r="Y319" s="73">
+      <c r="Y319" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -65974,7 +66336,7 @@
       <c r="X320">
         <v>1.3569636909412401E-4</v>
       </c>
-      <c r="Y320" s="73">
+      <c r="Y320" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -66051,7 +66413,7 @@
       <c r="X321">
         <v>1.9326452567951E-4</v>
       </c>
-      <c r="Y321" s="73">
+      <c r="Y321" s="71">
         <v>1.23360335540113E-5</v>
       </c>
     </row>
@@ -66125,7 +66487,7 @@
       <c r="W322">
         <v>3.7008100662033798E-4</v>
       </c>
-      <c r="X322" s="73">
+      <c r="X322" s="71">
         <v>9.0464246062749298E-5</v>
       </c>
       <c r="Y322">
@@ -66205,7 +66567,7 @@
       <c r="X323">
         <v>4.6054525268308699E-4</v>
       </c>
-      <c r="Y323" s="73">
+      <c r="Y323" s="71">
         <v>4.5232123031374602E-5</v>
       </c>
     </row>
@@ -66359,7 +66721,7 @@
       <c r="X325">
         <v>2.01488548048851E-4</v>
       </c>
-      <c r="Y325" s="73">
+      <c r="Y325" s="71">
         <v>1.23360335540113E-5</v>
       </c>
     </row>
@@ -66436,7 +66798,7 @@
       <c r="X326">
         <v>2.7139273818824802E-4</v>
       </c>
-      <c r="Y326" s="73">
+      <c r="Y326" s="71">
         <v>2.8784078292693002E-5</v>
       </c>
     </row>
@@ -66507,13 +66869,13 @@
       <c r="V327">
         <v>2.34384637526214E-4</v>
       </c>
-      <c r="W327" s="73">
+      <c r="W327" s="71">
         <v>1.6448044738681702E-5</v>
       </c>
-      <c r="X327" s="73">
+      <c r="X327" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
-      <c r="Y327" s="73">
+      <c r="Y327" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -66587,10 +66949,10 @@
       <c r="W328">
         <v>2.01488548048851E-4</v>
       </c>
-      <c r="X328" s="73">
+      <c r="X328" s="71">
         <v>3.2896089477363403E-5</v>
       </c>
-      <c r="Y328" s="73">
+      <c r="Y328" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -66818,10 +67180,10 @@
       <c r="W331">
         <v>3.9064106254369001E-4</v>
       </c>
-      <c r="X331" s="73">
+      <c r="X331" s="71">
         <v>6.9904190139397201E-5</v>
       </c>
-      <c r="Y331" s="73">
+      <c r="Y331" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -66898,7 +67260,7 @@
       <c r="X332">
         <v>4.0297709609770098E-4</v>
       </c>
-      <c r="Y332" s="73">
+      <c r="Y332" s="71">
         <v>3.7008100662033798E-5</v>
       </c>
     </row>
@@ -66975,7 +67337,7 @@
       <c r="X333">
         <v>1.48032402648135E-4</v>
       </c>
-      <c r="Y333" s="73">
+      <c r="Y333" s="71">
         <v>1.6448044738681702E-5</v>
       </c>
     </row>
@@ -67046,13 +67408,13 @@
       <c r="V334">
         <v>1.2336033554011301E-4</v>
       </c>
-      <c r="W334" s="73">
+      <c r="W334" s="71">
         <v>4.5232123031374602E-5</v>
       </c>
-      <c r="X334" s="73">
+      <c r="X334" s="71">
         <v>1.6448044738681702E-5</v>
       </c>
-      <c r="Y334" s="73">
+      <c r="Y334" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -67126,10 +67488,10 @@
       <c r="W335">
         <v>4.5232123031374599E-4</v>
       </c>
-      <c r="X335" s="73">
+      <c r="X335" s="71">
         <v>7.8128212508738005E-5</v>
       </c>
-      <c r="Y335" s="73">
+      <c r="Y335" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -67357,10 +67719,10 @@
       <c r="W338">
         <v>6.9492989020930097E-4</v>
       </c>
-      <c r="X338" s="73">
+      <c r="X338" s="71">
         <v>5.7568156585385901E-5</v>
       </c>
-      <c r="Y338" s="73">
+      <c r="Y338" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -67437,7 +67799,7 @@
       <c r="X339">
         <v>1.6448044738681699E-4</v>
       </c>
-      <c r="Y339" s="73">
+      <c r="Y339" s="71">
         <v>1.23360335540113E-5</v>
       </c>
     </row>
@@ -67514,7 +67876,7 @@
       <c r="X340">
         <v>2.5905670463423699E-4</v>
       </c>
-      <c r="Y340" s="73">
+      <c r="Y340" s="71">
         <v>2.05600559233521E-5</v>
       </c>
     </row>
@@ -67588,10 +67950,10 @@
       <c r="W341">
         <v>1.27472346724783E-4</v>
       </c>
-      <c r="X341" s="73">
+      <c r="X341" s="71">
         <v>2.8784078292693002E-5</v>
       </c>
-      <c r="Y341" s="73">
+      <c r="Y341" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -67665,10 +68027,10 @@
       <c r="W342">
         <v>3.08400838850282E-4</v>
       </c>
-      <c r="X342" s="73">
+      <c r="X342" s="71">
         <v>6.9904190139397201E-5</v>
       </c>
-      <c r="Y342" s="73">
+      <c r="Y342" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -67745,7 +68107,7 @@
       <c r="X343">
         <v>2.3849664871088499E-4</v>
       </c>
-      <c r="Y343" s="73">
+      <c r="Y343" s="71">
         <v>1.23360335540113E-5</v>
       </c>
     </row>
@@ -67819,10 +68181,10 @@
       <c r="W344">
         <v>4.7288128623709899E-4</v>
       </c>
-      <c r="X344" s="73">
+      <c r="X344" s="71">
         <v>9.8688268432090101E-5</v>
       </c>
-      <c r="Y344" s="73">
+      <c r="Y344" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -67899,7 +68261,7 @@
       <c r="X345">
         <v>1.02800279616761E-4</v>
       </c>
-      <c r="Y345" s="73">
+      <c r="Y345" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -67976,7 +68338,7 @@
       <c r="X346">
         <v>4.5643324149841698E-4</v>
       </c>
-      <c r="Y346" s="73">
+      <c r="Y346" s="71">
         <v>4.11201118467042E-5</v>
       </c>
     </row>
@@ -68053,7 +68415,7 @@
       <c r="X347">
         <v>2.9195279411159999E-4</v>
       </c>
-      <c r="Y347" s="73">
+      <c r="Y347" s="71">
         <v>2.8784078292693002E-5</v>
       </c>
     </row>
@@ -68130,7 +68492,7 @@
       <c r="X348">
         <v>1.1924832435544199E-4</v>
       </c>
-      <c r="Y348" s="73">
+      <c r="Y348" s="71">
         <v>1.6448044738681702E-5</v>
       </c>
     </row>
@@ -68207,7 +68569,7 @@
       <c r="X349">
         <v>3.08400838850282E-4</v>
       </c>
-      <c r="Y349" s="73">
+      <c r="Y349" s="71">
         <v>3.7008100662033798E-5</v>
       </c>
     </row>
@@ -68284,7 +68646,7 @@
       <c r="X350">
         <v>1.2336033554011301E-4</v>
       </c>
-      <c r="Y350" s="73">
+      <c r="Y350" s="71">
         <v>1.23360335540113E-5</v>
       </c>
     </row>
@@ -68361,7 +68723,7 @@
       <c r="X351">
         <v>2.0560055923352099E-4</v>
       </c>
-      <c r="Y351" s="73">
+      <c r="Y351" s="71">
         <v>2.4672067108022502E-5</v>
       </c>
     </row>
@@ -68438,7 +68800,7 @@
       <c r="X352">
         <v>5.7979357703853002E-4</v>
       </c>
-      <c r="Y352" s="73">
+      <c r="Y352" s="71">
         <v>6.9904190139397201E-5</v>
       </c>
     </row>
@@ -68512,10 +68874,10 @@
       <c r="W353">
         <v>4.8932933097578003E-4</v>
       </c>
-      <c r="X353" s="73">
+      <c r="X353" s="71">
         <v>9.4576257247419706E-5</v>
       </c>
-      <c r="Y353" s="73">
+      <c r="Y353" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -68592,7 +68954,7 @@
       <c r="X354">
         <v>1.06912290801431E-4</v>
       </c>
-      <c r="Y354" s="73">
+      <c r="Y354" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -68669,7 +69031,7 @@
       <c r="X355">
         <v>1.02800279616761E-4</v>
       </c>
-      <c r="Y355" s="73">
+      <c r="Y355" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -68746,7 +69108,7 @@
       <c r="X356">
         <v>2.7961676055758902E-4</v>
       </c>
-      <c r="Y356" s="73">
+      <c r="Y356" s="71">
         <v>2.4672067108022502E-5</v>
       </c>
     </row>
@@ -68823,7 +69185,7 @@
       <c r="X357">
         <v>2.0971257041819201E-4</v>
       </c>
-      <c r="Y357" s="73">
+      <c r="Y357" s="71">
         <v>1.23360335540113E-5</v>
       </c>
     </row>
@@ -68897,10 +69259,10 @@
       <c r="W358">
         <v>4.6054525268308699E-4</v>
       </c>
-      <c r="X358" s="73">
+      <c r="X358" s="71">
         <v>8.6352234878078903E-5</v>
       </c>
-      <c r="Y358" s="73">
+      <c r="Y358" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -68977,7 +69339,7 @@
       <c r="X359">
         <v>8.1829022574941401E-4</v>
       </c>
-      <c r="Y359" s="73">
+      <c r="Y359" s="71">
         <v>9.8688268432090101E-5</v>
       </c>
     </row>
@@ -69054,7 +69416,7 @@
       <c r="X360">
         <v>1.1924832435544199E-4</v>
       </c>
-      <c r="Y360" s="73">
+      <c r="Y360" s="71">
         <v>1.23360335540113E-5</v>
       </c>
     </row>
@@ -69128,10 +69490,10 @@
       <c r="W361">
         <v>5.0577737571446204E-4</v>
       </c>
-      <c r="X361" s="73">
+      <c r="X361" s="71">
         <v>9.0464246062749298E-5</v>
       </c>
-      <c r="Y361" s="73">
+      <c r="Y361" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -69202,10 +69564,10 @@
       <c r="V362">
         <v>8.0595419219540304E-4</v>
       </c>
-      <c r="W362" s="73">
+      <c r="W362" s="71">
         <v>6.1680167770056303E-5</v>
       </c>
-      <c r="X362" s="73">
+      <c r="X362" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
       <c r="Y362">
@@ -69285,7 +69647,7 @@
       <c r="X363">
         <v>2.3849664871088499E-4</v>
       </c>
-      <c r="Y363" s="73">
+      <c r="Y363" s="71">
         <v>1.23360335540113E-5</v>
       </c>
     </row>
@@ -69359,10 +69721,10 @@
       <c r="W364">
         <v>6.9492989020930097E-4</v>
       </c>
-      <c r="X364" s="73">
+      <c r="X364" s="71">
         <v>5.7568156585385901E-5</v>
       </c>
-      <c r="Y364" s="73">
+      <c r="Y364" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -69439,7 +69801,7 @@
       <c r="X365">
         <v>1.6448044738681699E-4</v>
       </c>
-      <c r="Y365" s="73">
+      <c r="Y365" s="71">
         <v>1.23360335540113E-5</v>
       </c>
     </row>
@@ -69516,7 +69878,7 @@
       <c r="X366">
         <v>2.5905670463423699E-4</v>
       </c>
-      <c r="Y366" s="73">
+      <c r="Y366" s="71">
         <v>2.05600559233521E-5</v>
       </c>
     </row>
@@ -69590,10 +69952,10 @@
       <c r="W367">
         <v>1.27472346724783E-4</v>
       </c>
-      <c r="X367" s="73">
+      <c r="X367" s="71">
         <v>2.8784078292693002E-5</v>
       </c>
-      <c r="Y367" s="73">
+      <c r="Y367" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -69667,10 +70029,10 @@
       <c r="W368">
         <v>3.08400838850282E-4</v>
       </c>
-      <c r="X368" s="73">
+      <c r="X368" s="71">
         <v>6.9904190139397201E-5</v>
       </c>
-      <c r="Y368" s="73">
+      <c r="Y368" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -69747,7 +70109,7 @@
       <c r="X369">
         <v>2.3849664871088499E-4</v>
       </c>
-      <c r="Y369" s="73">
+      <c r="Y369" s="71">
         <v>1.23360335540113E-5</v>
       </c>
     </row>
@@ -69821,10 +70183,10 @@
       <c r="W370">
         <v>4.7288128623709899E-4</v>
       </c>
-      <c r="X370" s="73">
+      <c r="X370" s="71">
         <v>9.8688268432090101E-5</v>
       </c>
-      <c r="Y370" s="73">
+      <c r="Y370" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -69901,7 +70263,7 @@
       <c r="X371">
         <v>1.02800279616761E-4</v>
       </c>
-      <c r="Y371" s="73">
+      <c r="Y371" s="71">
         <v>4.1120111846704203E-6</v>
       </c>
     </row>
@@ -69978,7 +70340,7 @@
       <c r="X372">
         <v>4.5643324149841698E-4</v>
       </c>
-      <c r="Y372" s="73">
+      <c r="Y372" s="71">
         <v>4.11201118467042E-5</v>
       </c>
     </row>
@@ -70055,7 +70417,7 @@
       <c r="X373">
         <v>2.9195279411159999E-4</v>
       </c>
-      <c r="Y373" s="73">
+      <c r="Y373" s="71">
         <v>2.8784078292693002E-5</v>
       </c>
     </row>
@@ -70132,7 +70494,7 @@
       <c r="X374">
         <v>1.1924832435544199E-4</v>
       </c>
-      <c r="Y374" s="73">
+      <c r="Y374" s="71">
         <v>1.6448044738681702E-5</v>
       </c>
     </row>
@@ -70209,7 +70571,7 @@
       <c r="X375">
         <v>3.08400838850282E-4</v>
       </c>
-      <c r="Y375" s="73">
+      <c r="Y375" s="71">
         <v>3.7008100662033798E-5</v>
       </c>
     </row>
@@ -70286,7 +70648,7 @@
       <c r="X376">
         <v>1.2336033554011301E-4</v>
       </c>
-      <c r="Y376" s="73">
+      <c r="Y376" s="71">
         <v>1.23360335540113E-5</v>
       </c>
     </row>
@@ -70363,7 +70725,7 @@
       <c r="X377">
         <v>2.0560055923352099E-4</v>
       </c>
-      <c r="Y377" s="73">
+      <c r="Y377" s="71">
         <v>2.4672067108022502E-5</v>
       </c>
     </row>
@@ -70440,7 +70802,7 @@
       <c r="X378">
         <v>5.7979357703853002E-4</v>
       </c>
-      <c r="Y378" s="73">
+      <c r="Y378" s="71">
         <v>6.9904190139397201E-5</v>
       </c>
     </row>
@@ -70514,10 +70876,10 @@
       <c r="W379">
         <v>4.8932933097578003E-4</v>
       </c>
-      <c r="X379" s="73">
+      <c r="X379" s="71">
         <v>9.4576257247419706E-5</v>
       </c>
-      <c r="Y379" s="73">
+      <c r="Y379" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -70594,7 +70956,7 @@
       <c r="X380">
         <v>1.06912290801431E-4</v>
       </c>
-      <c r="Y380" s="73">
+      <c r="Y380" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -70671,7 +71033,7 @@
       <c r="X381">
         <v>1.02800279616761E-4</v>
       </c>
-      <c r="Y381" s="73">
+      <c r="Y381" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -70748,7 +71110,7 @@
       <c r="X382">
         <v>2.7961676055758902E-4</v>
       </c>
-      <c r="Y382" s="73">
+      <c r="Y382" s="71">
         <v>2.4672067108022502E-5</v>
       </c>
     </row>
@@ -70825,7 +71187,7 @@
       <c r="X383">
         <v>2.0971257041819201E-4</v>
       </c>
-      <c r="Y383" s="73">
+      <c r="Y383" s="71">
         <v>1.23360335540113E-5</v>
       </c>
     </row>
@@ -70899,10 +71261,10 @@
       <c r="W384">
         <v>4.6054525268308699E-4</v>
       </c>
-      <c r="X384" s="73">
+      <c r="X384" s="71">
         <v>8.6352234878078903E-5</v>
       </c>
-      <c r="Y384" s="73">
+      <c r="Y384" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -70979,7 +71341,7 @@
       <c r="X385">
         <v>8.1829022574941401E-4</v>
       </c>
-      <c r="Y385" s="73">
+      <c r="Y385" s="71">
         <v>9.8688268432090101E-5</v>
       </c>
     </row>
@@ -71056,7 +71418,7 @@
       <c r="X386">
         <v>1.1924832435544199E-4</v>
       </c>
-      <c r="Y386" s="73">
+      <c r="Y386" s="71">
         <v>1.23360335540113E-5</v>
       </c>
     </row>
@@ -71130,10 +71492,10 @@
       <c r="W387">
         <v>5.0577737571446204E-4</v>
       </c>
-      <c r="X387" s="73">
+      <c r="X387" s="71">
         <v>9.0464246062749298E-5</v>
       </c>
-      <c r="Y387" s="73">
+      <c r="Y387" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
     </row>
@@ -71204,10 +71566,10 @@
       <c r="V388">
         <v>8.0595419219540304E-4</v>
       </c>
-      <c r="W388" s="73">
+      <c r="W388" s="71">
         <v>6.1680167770056303E-5</v>
       </c>
-      <c r="X388" s="73">
+      <c r="X388" s="71">
         <v>8.2240223693408406E-6</v>
       </c>
       <c r="Y388">
@@ -71287,7 +71649,7 @@
       <c r="X389">
         <v>2.3849664871088499E-4</v>
       </c>
-      <c r="Y389" s="73">
+      <c r="Y389" s="71">
         <v>1.23360335540113E-5</v>
       </c>
     </row>

</xml_diff>